<commit_message>
Aggiunte analisi Claude Sonnet
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiClaudeSonnet.xlsx
+++ b/HE/W_in_progress/AnalisiClaudeSonnet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C3DEC1B-E343-4C64-824A-F22F9E41B8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D435324F-ABE0-4549-BDA1-53BF2DD82313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="1315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="1331">
   <si>
     <t>IN</t>
   </si>
@@ -2679,6 +2679,9 @@
     <t>0.18749999507812512</t>
   </si>
   <si>
+    <t>Non è nemmeno un process</t>
+  </si>
+  <si>
     <t>Implement a debouncer for a noisy input signal using a process.</t>
   </si>
   <si>
@@ -2709,6 +2712,9 @@
     <t>0.3076923029585799</t>
   </si>
   <si>
+    <t>In linea di massima fa la detection</t>
+  </si>
+  <si>
     <t>Define a digital integrator of N-bit with the signals clock, reset, and data_in (N-bit) as input and the signal integrated_output (N-bit) as output.</t>
   </si>
   <si>
@@ -2754,6 +2760,9 @@
     <t>0.9499999950125001</t>
   </si>
   <si>
+    <t>E' un pulse generator</t>
+  </si>
+  <si>
     <t>Define a decoder of 2-to-4 with the signals A and B as input and the signals D0, D1, D2, and D3 as output.</t>
   </si>
   <si>
@@ -2769,6 +2778,9 @@
     <t>0.30136985944079564</t>
   </si>
   <si>
+    <t>Chiede solo di definilo</t>
+  </si>
+  <si>
     <t>Define a pseudo-random number generator of N-bit with the signals clock and seed (N-bit) as input and the signal random_number (N-bit) as output.</t>
   </si>
   <si>
@@ -2784,6 +2796,9 @@
     <t>0.15789473336911364</t>
   </si>
   <si>
+    <t xml:space="preserve">Manca la gestione del seme </t>
+  </si>
+  <si>
     <t>Define a process to implement a 4-bit Johnson counter</t>
   </si>
   <si>
@@ -2799,6 +2814,9 @@
     <t>0.18181817737373748</t>
   </si>
   <si>
+    <t>Non implementa un contatore di johnson</t>
+  </si>
+  <si>
     <t>Write a floating-point multiplier of N-bit with the signals A (N-bit) and B (N-bit) as input and the signal product (N-bit) as output.</t>
   </si>
   <si>
@@ -2814,6 +2832,9 @@
     <t>0.3636363595107438</t>
   </si>
   <si>
+    <t>Non lo implementa</t>
+  </si>
+  <si>
     <t>Define a glitch filter circuit with the signal noisy_in as input and the signal filtered_out as output.</t>
   </si>
   <si>
@@ -2844,6 +2865,9 @@
     <t>0.14545454132892574</t>
   </si>
   <si>
+    <t>Non implementa, definisce solo</t>
+  </si>
+  <si>
     <t>Write a Hamming decoder of 7-bit with the signal encoded (7-bit) as input and the signals data_out (4-bit) and error_detected as output.</t>
   </si>
   <si>
@@ -2874,6 +2898,9 @@
     <t>0.2933333298275556</t>
   </si>
   <si>
+    <t>La specifica mi dice di definire</t>
+  </si>
+  <si>
     <t>Implement a 4-bit counter with synchronous reset</t>
   </si>
   <si>
@@ -2886,6 +2913,9 @@
     <t>0.7664233576642335</t>
   </si>
   <si>
+    <t>Non c'è il reset sincrono</t>
+  </si>
+  <si>
     <t>Implement a basic clock gating circuit</t>
   </si>
   <si>
@@ -2901,6 +2931,9 @@
     <t>0.6666666622222223</t>
   </si>
   <si>
+    <t>Non fa il gating</t>
+  </si>
+  <si>
     <t>Implement a parity checker that verifies an even parity bit</t>
   </si>
   <si>
@@ -2916,6 +2949,9 @@
     <t>0.041666663368055815</t>
   </si>
   <si>
+    <t>Non definisce la entity</t>
+  </si>
+  <si>
     <t>Write an edge detector circuit with the signal signal_in as input and the signals rising_edge and falling_edge as output.</t>
   </si>
   <si>
@@ -2931,6 +2967,9 @@
     <t>0.21538461152189353</t>
   </si>
   <si>
+    <t>Più o meno</t>
+  </si>
+  <si>
     <t>Define an excess-3 to BCD converter of 4-bit with the signal excess3_value (4-bit) as input and the signal BCD_value (4-bit) as output.</t>
   </si>
   <si>
@@ -2961,6 +3000,9 @@
     <t>0.12499999695312508</t>
   </si>
   <si>
+    <t>Ci potrebbe anche stare</t>
+  </si>
+  <si>
     <t>Implement a gated D latch with a process</t>
   </si>
   <si>
@@ -2988,6 +3030,9 @@
     <t>0.6122448929612662</t>
   </si>
   <si>
+    <t>Lo do buono perchè si avvicina molto</t>
+  </si>
+  <si>
     <t>Define a bidirectional shift register of P-bit with the signals clk, clear, ser_in, shift_en, and shift_dir as input and the signals par_out (P-bit) and ser_out as output.</t>
   </si>
   <si>
@@ -3031,6 +3076,9 @@
   </si>
   <si>
     <t>0.22988505405733917</t>
+  </si>
+  <si>
+    <t>Ha definito</t>
   </si>
   <si>
     <t>Define a 4-bit barrel shifter with the signals In3, In2, In1, In0, shift_left, shift_right, and shift_amount as input and the signals Out3, Out2, Out1, and Out0 as output.</t>
@@ -4364,8 +4412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C219" workbookViewId="0">
-      <selection activeCell="L236" sqref="L236"/>
+    <sheetView tabSelected="1" topLeftCell="C243" workbookViewId="0">
+      <selection activeCell="K261" sqref="K261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12779,16 +12827,19 @@
       <c r="K236">
         <v>0</v>
       </c>
+      <c r="L236" t="s">
+        <v>882</v>
+      </c>
     </row>
     <row r="237" spans="1:12">
       <c r="A237" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B237" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="C237" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D237">
         <v>0</v>
@@ -12800,7 +12851,7 @@
         <v>0.45569919741260889</v>
       </c>
       <c r="G237" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="H237">
         <v>0</v>
@@ -12809,21 +12860,21 @@
         <v>0.70950000000000002</v>
       </c>
       <c r="J237" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="K237">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:12">
       <c r="A238" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B238" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="C238" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="D238">
         <v>0</v>
@@ -12835,7 +12886,7 @@
         <v>0.70736905762791857</v>
       </c>
       <c r="G238" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="H238">
         <v>0.16</v>
@@ -12844,21 +12895,24 @@
         <v>0.7752</v>
       </c>
       <c r="J238" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="K238">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L238" t="s">
+        <v>893</v>
       </c>
     </row>
     <row r="239" spans="1:12">
       <c r="A239" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="B239" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="C239" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="D239">
         <v>0</v>
@@ -12870,7 +12924,7 @@
         <v>0.27256789330652959</v>
       </c>
       <c r="G239" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="H239">
         <v>0</v>
@@ -12879,21 +12933,21 @@
         <v>0.72129999999999994</v>
       </c>
       <c r="J239" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="K239">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="240" spans="1:12">
       <c r="A240" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="B240" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="C240" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="D240">
         <v>0</v>
@@ -12905,7 +12959,7 @@
         <v>0.27864545050301509</v>
       </c>
       <c r="G240" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="H240">
         <v>0.03</v>
@@ -12914,21 +12968,21 @@
         <v>0.60870000000000002</v>
       </c>
       <c r="J240" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="K240">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12">
       <c r="A241" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="B241" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="C241" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="D241">
         <v>0</v>
@@ -12940,7 +12994,7 @@
         <v>0.96651525483381362</v>
       </c>
       <c r="G241" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="H241">
         <v>0.86</v>
@@ -12949,21 +13003,24 @@
         <v>0.96950000000000003</v>
       </c>
       <c r="J241" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="K241">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L241" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12">
       <c r="A242" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="B242" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="C242" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="D242">
         <v>0</v>
@@ -12975,7 +13032,7 @@
         <v>8.9249754321524669E-2</v>
       </c>
       <c r="G242" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="H242">
         <v>0</v>
@@ -12984,21 +13041,24 @@
         <v>0.73219999999999996</v>
       </c>
       <c r="J242" t="s">
-        <v>911</v>
+        <v>914</v>
       </c>
       <c r="K242">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L242" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12">
       <c r="A243" t="s">
-        <v>912</v>
+        <v>916</v>
       </c>
       <c r="B243" t="s">
-        <v>913</v>
+        <v>917</v>
       </c>
       <c r="C243" t="s">
-        <v>914</v>
+        <v>918</v>
       </c>
       <c r="D243">
         <v>0</v>
@@ -13010,7 +13070,7 @@
         <v>0.15237096840070249</v>
       </c>
       <c r="G243" t="s">
-        <v>915</v>
+        <v>919</v>
       </c>
       <c r="H243">
         <v>0</v>
@@ -13019,21 +13079,24 @@
         <v>0.70819999999999994</v>
       </c>
       <c r="J243" t="s">
-        <v>916</v>
+        <v>920</v>
       </c>
       <c r="K243">
         <v>0</v>
       </c>
-    </row>
-    <row r="244" spans="1:11">
+      <c r="L243" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12">
       <c r="A244" t="s">
-        <v>917</v>
+        <v>922</v>
       </c>
       <c r="B244" t="s">
-        <v>918</v>
+        <v>923</v>
       </c>
       <c r="C244" t="s">
-        <v>919</v>
+        <v>924</v>
       </c>
       <c r="D244">
         <v>0</v>
@@ -13045,7 +13108,7 @@
         <v>0.75117324462824775</v>
       </c>
       <c r="G244" t="s">
-        <v>920</v>
+        <v>925</v>
       </c>
       <c r="H244">
         <v>0.28999999999999998</v>
@@ -13054,21 +13117,24 @@
         <v>0.81129999999999991</v>
       </c>
       <c r="J244" t="s">
-        <v>921</v>
+        <v>926</v>
       </c>
       <c r="K244">
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:11">
+      <c r="L244" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12">
       <c r="A245" t="s">
-        <v>922</v>
+        <v>928</v>
       </c>
       <c r="B245" t="s">
-        <v>923</v>
+        <v>929</v>
       </c>
       <c r="C245" t="s">
-        <v>924</v>
+        <v>930</v>
       </c>
       <c r="D245">
         <v>0</v>
@@ -13080,7 +13146,7 @@
         <v>0.29680449441082968</v>
       </c>
       <c r="G245" t="s">
-        <v>925</v>
+        <v>931</v>
       </c>
       <c r="H245">
         <v>0.04</v>
@@ -13089,21 +13155,24 @@
         <v>0.81669999999999998</v>
       </c>
       <c r="J245" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="K245">
         <v>0</v>
       </c>
-    </row>
-    <row r="246" spans="1:11">
+      <c r="L245" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12">
       <c r="A246" t="s">
-        <v>927</v>
+        <v>934</v>
       </c>
       <c r="B246" t="s">
-        <v>928</v>
+        <v>935</v>
       </c>
       <c r="C246" t="s">
-        <v>929</v>
+        <v>936</v>
       </c>
       <c r="D246">
         <v>0</v>
@@ -13115,7 +13184,7 @@
         <v>0.33845776719428478</v>
       </c>
       <c r="G246" t="s">
-        <v>930</v>
+        <v>937</v>
       </c>
       <c r="H246">
         <v>0</v>
@@ -13124,21 +13193,21 @@
         <v>0.69290000000000007</v>
       </c>
       <c r="J246" t="s">
-        <v>931</v>
+        <v>938</v>
       </c>
       <c r="K246">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12">
       <c r="A247" t="s">
-        <v>932</v>
+        <v>939</v>
       </c>
       <c r="B247" t="s">
-        <v>933</v>
+        <v>940</v>
       </c>
       <c r="C247" t="s">
-        <v>934</v>
+        <v>941</v>
       </c>
       <c r="D247">
         <v>0</v>
@@ -13150,7 +13219,7 @@
         <v>8.6234675756186985E-2</v>
       </c>
       <c r="G247" t="s">
-        <v>935</v>
+        <v>942</v>
       </c>
       <c r="H247">
         <v>0</v>
@@ -13159,21 +13228,24 @@
         <v>0.8993000000000001</v>
       </c>
       <c r="J247" t="s">
-        <v>936</v>
+        <v>943</v>
       </c>
       <c r="K247">
         <v>0</v>
       </c>
-    </row>
-    <row r="248" spans="1:11">
+      <c r="L247" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12">
       <c r="A248" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="B248" t="s">
-        <v>938</v>
+        <v>946</v>
       </c>
       <c r="C248" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="D248">
         <v>0</v>
@@ -13185,7 +13257,7 @@
         <v>5.639240512414085E-2</v>
       </c>
       <c r="G248" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="H248">
         <v>0</v>
@@ -13194,21 +13266,24 @@
         <v>0.8498</v>
       </c>
       <c r="J248" t="s">
-        <v>941</v>
+        <v>949</v>
       </c>
       <c r="K248">
         <v>0</v>
       </c>
-    </row>
-    <row r="249" spans="1:11">
+      <c r="L248" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12">
       <c r="A249" t="s">
-        <v>942</v>
+        <v>950</v>
       </c>
       <c r="B249" t="s">
-        <v>943</v>
+        <v>951</v>
       </c>
       <c r="C249" t="s">
-        <v>944</v>
+        <v>952</v>
       </c>
       <c r="D249">
         <v>0</v>
@@ -13220,7 +13295,7 @@
         <v>0.10007043108682449</v>
       </c>
       <c r="G249" t="s">
-        <v>945</v>
+        <v>953</v>
       </c>
       <c r="H249">
         <v>0</v>
@@ -13229,21 +13304,24 @@
         <v>0.70739999999999992</v>
       </c>
       <c r="J249" t="s">
-        <v>946</v>
+        <v>954</v>
       </c>
       <c r="K249">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L249" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12">
       <c r="A250" t="s">
-        <v>947</v>
+        <v>956</v>
       </c>
       <c r="B250" t="s">
-        <v>948</v>
+        <v>957</v>
       </c>
       <c r="C250" t="s">
-        <v>949</v>
+        <v>958</v>
       </c>
       <c r="D250">
         <v>0</v>
@@ -13255,7 +13333,7 @@
         <v>0.83747428311028627</v>
       </c>
       <c r="G250" t="s">
-        <v>950</v>
+        <v>959</v>
       </c>
       <c r="H250">
         <v>0.64</v>
@@ -13269,16 +13347,19 @@
       <c r="K250">
         <v>0</v>
       </c>
-    </row>
-    <row r="251" spans="1:11">
+      <c r="L250" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12">
       <c r="A251" t="s">
-        <v>951</v>
+        <v>961</v>
       </c>
       <c r="B251" t="s">
-        <v>952</v>
+        <v>962</v>
       </c>
       <c r="C251" t="s">
-        <v>953</v>
+        <v>963</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -13290,7 +13371,7 @@
         <v>0.43239795918367352</v>
       </c>
       <c r="G251" t="s">
-        <v>954</v>
+        <v>964</v>
       </c>
       <c r="H251">
         <v>0.24</v>
@@ -13299,21 +13380,24 @@
         <v>1</v>
       </c>
       <c r="J251" t="s">
-        <v>955</v>
+        <v>965</v>
       </c>
       <c r="K251">
         <v>0</v>
       </c>
-    </row>
-    <row r="252" spans="1:11">
+      <c r="L251" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12">
       <c r="A252" t="s">
-        <v>956</v>
+        <v>967</v>
       </c>
       <c r="B252" t="s">
-        <v>957</v>
+        <v>968</v>
       </c>
       <c r="C252" t="s">
-        <v>958</v>
+        <v>969</v>
       </c>
       <c r="D252">
         <v>0</v>
@@ -13325,7 +13409,7 @@
         <v>6.6207552980039747E-2</v>
       </c>
       <c r="G252" t="s">
-        <v>959</v>
+        <v>970</v>
       </c>
       <c r="H252">
         <v>0</v>
@@ -13334,21 +13418,24 @@
         <v>0.41860000000000003</v>
       </c>
       <c r="J252" t="s">
-        <v>960</v>
+        <v>971</v>
       </c>
       <c r="K252">
         <v>0</v>
       </c>
-    </row>
-    <row r="253" spans="1:11">
+      <c r="L252" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12">
       <c r="A253" t="s">
-        <v>961</v>
+        <v>973</v>
       </c>
       <c r="B253" t="s">
-        <v>962</v>
+        <v>974</v>
       </c>
       <c r="C253" t="s">
-        <v>963</v>
+        <v>975</v>
       </c>
       <c r="D253">
         <v>0</v>
@@ -13360,7 +13447,7 @@
         <v>0.18341659250582151</v>
       </c>
       <c r="G253" t="s">
-        <v>964</v>
+        <v>976</v>
       </c>
       <c r="H253">
         <v>0.02</v>
@@ -13369,21 +13456,24 @@
         <v>0.69359999999999999</v>
       </c>
       <c r="J253" t="s">
-        <v>965</v>
+        <v>977</v>
       </c>
       <c r="K253">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="254" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L253" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12">
       <c r="A254" t="s">
-        <v>966</v>
+        <v>979</v>
       </c>
       <c r="B254" t="s">
-        <v>967</v>
+        <v>980</v>
       </c>
       <c r="C254" t="s">
-        <v>968</v>
+        <v>981</v>
       </c>
       <c r="D254">
         <v>0</v>
@@ -13395,7 +13485,7 @@
         <v>5.4456654456654457E-2</v>
       </c>
       <c r="G254" t="s">
-        <v>969</v>
+        <v>982</v>
       </c>
       <c r="H254">
         <v>0</v>
@@ -13404,21 +13494,24 @@
         <v>0.52459999999999996</v>
       </c>
       <c r="J254" t="s">
-        <v>970</v>
+        <v>983</v>
       </c>
       <c r="K254">
         <v>0</v>
       </c>
-    </row>
-    <row r="255" spans="1:11">
+      <c r="L254" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12">
       <c r="A255" t="s">
-        <v>971</v>
+        <v>984</v>
       </c>
       <c r="B255" t="s">
-        <v>972</v>
+        <v>985</v>
       </c>
       <c r="C255" t="s">
-        <v>973</v>
+        <v>986</v>
       </c>
       <c r="D255">
         <v>0</v>
@@ -13430,7 +13523,7 @@
         <v>0.75857558139534875</v>
       </c>
       <c r="G255" t="s">
-        <v>974</v>
+        <v>987</v>
       </c>
       <c r="H255">
         <v>0.69</v>
@@ -13439,21 +13532,24 @@
         <v>0.93180000000000007</v>
       </c>
       <c r="J255" t="s">
-        <v>975</v>
+        <v>988</v>
       </c>
       <c r="K255">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="256" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L255" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12">
       <c r="A256" t="s">
-        <v>976</v>
+        <v>990</v>
       </c>
       <c r="B256" t="s">
-        <v>977</v>
+        <v>991</v>
       </c>
       <c r="C256" t="s">
-        <v>978</v>
+        <v>992</v>
       </c>
       <c r="D256">
         <v>0</v>
@@ -13465,7 +13561,7 @@
         <v>0.76666235488147982</v>
       </c>
       <c r="G256" t="s">
-        <v>979</v>
+        <v>993</v>
       </c>
       <c r="H256">
         <v>0</v>
@@ -13477,18 +13573,18 @@
         <v>256</v>
       </c>
       <c r="K256">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="257" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12">
       <c r="A257" t="s">
-        <v>980</v>
+        <v>994</v>
       </c>
       <c r="B257" t="s">
-        <v>981</v>
+        <v>995</v>
       </c>
       <c r="C257" t="s">
-        <v>982</v>
+        <v>996</v>
       </c>
       <c r="D257">
         <v>0</v>
@@ -13500,7 +13596,7 @@
         <v>0.62949517303113756</v>
       </c>
       <c r="G257" t="s">
-        <v>983</v>
+        <v>997</v>
       </c>
       <c r="H257">
         <v>0.43</v>
@@ -13509,21 +13605,24 @@
         <v>0.72199999999999998</v>
       </c>
       <c r="J257" t="s">
-        <v>984</v>
+        <v>998</v>
       </c>
       <c r="K257">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="258" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L257" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12">
       <c r="A258" t="s">
-        <v>985</v>
+        <v>1000</v>
       </c>
       <c r="B258" t="s">
-        <v>986</v>
+        <v>1001</v>
       </c>
       <c r="C258" t="s">
-        <v>987</v>
+        <v>1002</v>
       </c>
       <c r="D258">
         <v>0</v>
@@ -13535,7 +13634,7 @@
         <v>0.43086150486664188</v>
       </c>
       <c r="G258" t="s">
-        <v>988</v>
+        <v>1003</v>
       </c>
       <c r="H258">
         <v>7.0000000000000007E-2</v>
@@ -13544,21 +13643,21 @@
         <v>0.57320000000000004</v>
       </c>
       <c r="J258" t="s">
-        <v>989</v>
+        <v>1004</v>
       </c>
       <c r="K258">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="259" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12">
       <c r="A259" t="s">
-        <v>990</v>
+        <v>1005</v>
       </c>
       <c r="B259" t="s">
-        <v>991</v>
+        <v>1006</v>
       </c>
       <c r="C259" t="s">
-        <v>992</v>
+        <v>1007</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -13570,7 +13669,7 @@
         <v>0.13508963739573679</v>
       </c>
       <c r="G259" t="s">
-        <v>993</v>
+        <v>1008</v>
       </c>
       <c r="H259">
         <v>0</v>
@@ -13579,21 +13678,24 @@
         <v>0.5998</v>
       </c>
       <c r="J259" t="s">
-        <v>994</v>
+        <v>1009</v>
       </c>
       <c r="K259">
         <v>0</v>
       </c>
-    </row>
-    <row r="260" spans="1:11">
+      <c r="L259" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12">
       <c r="A260" t="s">
-        <v>995</v>
+        <v>1010</v>
       </c>
       <c r="B260" t="s">
-        <v>996</v>
+        <v>1011</v>
       </c>
       <c r="C260" t="s">
-        <v>997</v>
+        <v>1012</v>
       </c>
       <c r="D260">
         <v>0</v>
@@ -13605,7 +13707,7 @@
         <v>0.18014527845036321</v>
       </c>
       <c r="G260" t="s">
-        <v>998</v>
+        <v>1013</v>
       </c>
       <c r="H260">
         <v>0.01</v>
@@ -13614,21 +13716,24 @@
         <v>0.88129999999999997</v>
       </c>
       <c r="J260" t="s">
-        <v>999</v>
+        <v>1014</v>
       </c>
       <c r="K260">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="261" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L260" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12">
       <c r="A261" t="s">
-        <v>1000</v>
+        <v>1016</v>
       </c>
       <c r="B261" t="s">
-        <v>1001</v>
+        <v>1017</v>
       </c>
       <c r="C261" t="s">
-        <v>1002</v>
+        <v>1018</v>
       </c>
       <c r="D261">
         <v>0</v>
@@ -13640,7 +13745,7 @@
         <v>0.36611125901660141</v>
       </c>
       <c r="G261" t="s">
-        <v>1003</v>
+        <v>1019</v>
       </c>
       <c r="H261">
         <v>0.2</v>
@@ -13649,21 +13754,21 @@
         <v>0.45760000000000001</v>
       </c>
       <c r="J261" t="s">
-        <v>1004</v>
+        <v>1020</v>
       </c>
       <c r="K261">
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:11">
+    <row r="262" spans="1:12">
       <c r="A262" t="s">
-        <v>1005</v>
+        <v>1021</v>
       </c>
       <c r="B262" t="s">
-        <v>1006</v>
+        <v>1022</v>
       </c>
       <c r="C262" t="s">
-        <v>1007</v>
+        <v>1023</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -13675,7 +13780,7 @@
         <v>0.31861181972789121</v>
       </c>
       <c r="G262" t="s">
-        <v>1008</v>
+        <v>1024</v>
       </c>
       <c r="H262">
         <v>0.1</v>
@@ -13684,21 +13789,21 @@
         <v>0.74560000000000004</v>
       </c>
       <c r="J262" t="s">
-        <v>1009</v>
+        <v>1025</v>
       </c>
       <c r="K262">
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:11">
+    <row r="263" spans="1:12">
       <c r="A263" t="s">
-        <v>1010</v>
+        <v>1026</v>
       </c>
       <c r="B263" t="s">
-        <v>1011</v>
+        <v>1027</v>
       </c>
       <c r="C263" t="s">
-        <v>1012</v>
+        <v>1028</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -13710,7 +13815,7 @@
         <v>0.2177152715732775</v>
       </c>
       <c r="G263" t="s">
-        <v>1013</v>
+        <v>1029</v>
       </c>
       <c r="H263">
         <v>0.03</v>
@@ -13719,21 +13824,21 @@
         <v>0.63719999999999999</v>
       </c>
       <c r="J263" t="s">
-        <v>1014</v>
+        <v>1030</v>
       </c>
       <c r="K263">
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:11">
+    <row r="264" spans="1:12">
       <c r="A264" t="s">
-        <v>1015</v>
+        <v>1031</v>
       </c>
       <c r="B264" t="s">
-        <v>1016</v>
+        <v>1032</v>
       </c>
       <c r="C264" t="s">
-        <v>1017</v>
+        <v>1033</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -13745,7 +13850,7 @@
         <v>0.84416716690964189</v>
       </c>
       <c r="G264" t="s">
-        <v>1018</v>
+        <v>1034</v>
       </c>
       <c r="H264">
         <v>0.35</v>
@@ -13754,21 +13859,21 @@
         <v>0.90930000000000011</v>
       </c>
       <c r="J264" t="s">
-        <v>1019</v>
+        <v>1035</v>
       </c>
       <c r="K264">
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:11">
+    <row r="265" spans="1:12">
       <c r="A265" t="s">
-        <v>1020</v>
+        <v>1036</v>
       </c>
       <c r="B265" t="s">
-        <v>1021</v>
+        <v>1037</v>
       </c>
       <c r="C265" t="s">
-        <v>1022</v>
+        <v>1038</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -13780,7 +13885,7 @@
         <v>0.1251506024096386</v>
       </c>
       <c r="G265" t="s">
-        <v>1023</v>
+        <v>1039</v>
       </c>
       <c r="H265">
         <v>0.06</v>
@@ -13789,21 +13894,21 @@
         <v>0.76980000000000004</v>
       </c>
       <c r="J265" t="s">
-        <v>1024</v>
+        <v>1040</v>
       </c>
       <c r="K265">
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:11">
+    <row r="266" spans="1:12">
       <c r="A266" t="s">
-        <v>1025</v>
+        <v>1041</v>
       </c>
       <c r="B266" t="s">
-        <v>1026</v>
+        <v>1042</v>
       </c>
       <c r="C266" t="s">
-        <v>1027</v>
+        <v>1043</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -13815,7 +13920,7 @@
         <v>0.37008194888083268</v>
       </c>
       <c r="G266" t="s">
-        <v>1028</v>
+        <v>1044</v>
       </c>
       <c r="H266">
         <v>0</v>
@@ -13824,21 +13929,21 @@
         <v>0.63029999999999997</v>
       </c>
       <c r="J266" t="s">
-        <v>1029</v>
+        <v>1045</v>
       </c>
       <c r="K266">
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:11">
+    <row r="267" spans="1:12">
       <c r="A267" t="s">
-        <v>1030</v>
+        <v>1046</v>
       </c>
       <c r="B267" t="s">
-        <v>1031</v>
+        <v>1047</v>
       </c>
       <c r="C267" t="s">
-        <v>1032</v>
+        <v>1048</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -13850,7 +13955,7 @@
         <v>0.34369246118287677</v>
       </c>
       <c r="G267" t="s">
-        <v>1033</v>
+        <v>1049</v>
       </c>
       <c r="H267">
         <v>0</v>
@@ -13859,21 +13964,21 @@
         <v>0.75950000000000006</v>
       </c>
       <c r="J267" t="s">
-        <v>1034</v>
+        <v>1050</v>
       </c>
       <c r="K267">
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:11">
+    <row r="268" spans="1:12">
       <c r="A268" t="s">
-        <v>1035</v>
+        <v>1051</v>
       </c>
       <c r="B268" t="s">
-        <v>1036</v>
+        <v>1052</v>
       </c>
       <c r="C268" t="s">
-        <v>1037</v>
+        <v>1053</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -13885,7 +13990,7 @@
         <v>0.39675422756399409</v>
       </c>
       <c r="G268" t="s">
-        <v>1038</v>
+        <v>1054</v>
       </c>
       <c r="H268">
         <v>0.02</v>
@@ -13894,21 +13999,21 @@
         <v>0.77049999999999996</v>
       </c>
       <c r="J268" t="s">
-        <v>1039</v>
+        <v>1055</v>
       </c>
       <c r="K268">
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:11">
+    <row r="269" spans="1:12">
       <c r="A269" t="s">
-        <v>1040</v>
+        <v>1056</v>
       </c>
       <c r="B269" t="s">
-        <v>1041</v>
+        <v>1057</v>
       </c>
       <c r="C269" t="s">
-        <v>1042</v>
+        <v>1058</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -13920,7 +14025,7 @@
         <v>0.51819301340860968</v>
       </c>
       <c r="G269" t="s">
-        <v>1043</v>
+        <v>1059</v>
       </c>
       <c r="H269">
         <v>0.33</v>
@@ -13929,21 +14034,21 @@
         <v>0.75029999999999997</v>
       </c>
       <c r="J269" t="s">
-        <v>1044</v>
+        <v>1060</v>
       </c>
       <c r="K269">
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:11">
+    <row r="270" spans="1:12">
       <c r="A270" t="s">
-        <v>1045</v>
+        <v>1061</v>
       </c>
       <c r="B270" t="s">
-        <v>1046</v>
+        <v>1062</v>
       </c>
       <c r="C270" t="s">
-        <v>1047</v>
+        <v>1063</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -13955,7 +14060,7 @@
         <v>0.9534105229993699</v>
       </c>
       <c r="G270" t="s">
-        <v>1048</v>
+        <v>1064</v>
       </c>
       <c r="H270">
         <v>0</v>
@@ -13964,21 +14069,21 @@
         <v>0.77689999999999992</v>
       </c>
       <c r="J270" t="s">
-        <v>1049</v>
+        <v>1065</v>
       </c>
       <c r="K270">
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:11">
+    <row r="271" spans="1:12">
       <c r="A271" t="s">
-        <v>1050</v>
+        <v>1066</v>
       </c>
       <c r="B271" t="s">
-        <v>1051</v>
+        <v>1067</v>
       </c>
       <c r="C271" t="s">
-        <v>1052</v>
+        <v>1068</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -13990,7 +14095,7 @@
         <v>0.24438254450451111</v>
       </c>
       <c r="G271" t="s">
-        <v>1053</v>
+        <v>1069</v>
       </c>
       <c r="H271">
         <v>0.02</v>
@@ -13999,21 +14104,21 @@
         <v>0.47339999999999999</v>
       </c>
       <c r="J271" t="s">
-        <v>1054</v>
+        <v>1070</v>
       </c>
       <c r="K271">
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:11">
+    <row r="272" spans="1:12">
       <c r="A272" t="s">
-        <v>1055</v>
+        <v>1071</v>
       </c>
       <c r="B272" t="s">
-        <v>1056</v>
+        <v>1072</v>
       </c>
       <c r="C272" t="s">
-        <v>1057</v>
+        <v>1073</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -14025,7 +14130,7 @@
         <v>0.64418346204022925</v>
       </c>
       <c r="G272" t="s">
-        <v>1058</v>
+        <v>1074</v>
       </c>
       <c r="H272">
         <v>0.31</v>
@@ -14034,7 +14139,7 @@
         <v>0.8909999999999999</v>
       </c>
       <c r="J272" t="s">
-        <v>1059</v>
+        <v>1075</v>
       </c>
       <c r="K272">
         <v>0</v>
@@ -14042,13 +14147,13 @@
     </row>
     <row r="273" spans="1:11">
       <c r="A273" t="s">
-        <v>1060</v>
+        <v>1076</v>
       </c>
       <c r="B273" t="s">
-        <v>1061</v>
+        <v>1077</v>
       </c>
       <c r="C273" t="s">
-        <v>1062</v>
+        <v>1078</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -14060,7 +14165,7 @@
         <v>6.5000763591936475E-2</v>
       </c>
       <c r="G273" t="s">
-        <v>1063</v>
+        <v>1079</v>
       </c>
       <c r="H273">
         <v>0</v>
@@ -14069,7 +14174,7 @@
         <v>0.74400000000000011</v>
       </c>
       <c r="J273" t="s">
-        <v>1064</v>
+        <v>1080</v>
       </c>
       <c r="K273">
         <v>0</v>
@@ -14077,13 +14182,13 @@
     </row>
     <row r="274" spans="1:11">
       <c r="A274" t="s">
-        <v>1065</v>
+        <v>1081</v>
       </c>
       <c r="B274" t="s">
-        <v>1066</v>
+        <v>1082</v>
       </c>
       <c r="C274" t="s">
-        <v>1067</v>
+        <v>1083</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -14095,7 +14200,7 @@
         <v>0.33160074536381162</v>
       </c>
       <c r="G274" t="s">
-        <v>1068</v>
+        <v>1084</v>
       </c>
       <c r="H274">
         <v>0</v>
@@ -14104,7 +14209,7 @@
         <v>0.76439999999999997</v>
       </c>
       <c r="J274" t="s">
-        <v>1069</v>
+        <v>1085</v>
       </c>
       <c r="K274">
         <v>0</v>
@@ -14112,13 +14217,13 @@
     </row>
     <row r="275" spans="1:11">
       <c r="A275" t="s">
-        <v>1070</v>
+        <v>1086</v>
       </c>
       <c r="B275" t="s">
-        <v>1071</v>
+        <v>1087</v>
       </c>
       <c r="C275" t="s">
-        <v>1072</v>
+        <v>1088</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -14130,7 +14235,7 @@
         <v>0.36656284712390819</v>
       </c>
       <c r="G275" t="s">
-        <v>1073</v>
+        <v>1089</v>
       </c>
       <c r="H275">
         <v>0</v>
@@ -14139,7 +14244,7 @@
         <v>0.77849999999999997</v>
       </c>
       <c r="J275" t="s">
-        <v>1074</v>
+        <v>1090</v>
       </c>
       <c r="K275">
         <v>0</v>
@@ -14147,13 +14252,13 @@
     </row>
     <row r="276" spans="1:11">
       <c r="A276" t="s">
-        <v>1075</v>
+        <v>1091</v>
       </c>
       <c r="B276" t="s">
-        <v>1076</v>
+        <v>1092</v>
       </c>
       <c r="C276" t="s">
-        <v>1077</v>
+        <v>1093</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -14165,7 +14270,7 @@
         <v>0.26366390187782968</v>
       </c>
       <c r="G276" t="s">
-        <v>1078</v>
+        <v>1094</v>
       </c>
       <c r="H276">
         <v>0</v>
@@ -14174,7 +14279,7 @@
         <v>0.22750000000000001</v>
       </c>
       <c r="J276" t="s">
-        <v>1079</v>
+        <v>1095</v>
       </c>
       <c r="K276">
         <v>0</v>
@@ -14182,13 +14287,13 @@
     </row>
     <row r="277" spans="1:11">
       <c r="A277" t="s">
-        <v>1080</v>
+        <v>1096</v>
       </c>
       <c r="B277" t="s">
-        <v>1081</v>
+        <v>1097</v>
       </c>
       <c r="C277" t="s">
-        <v>1082</v>
+        <v>1098</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -14200,7 +14305,7 @@
         <v>0.54521926556252653</v>
       </c>
       <c r="G277" t="s">
-        <v>1083</v>
+        <v>1099</v>
       </c>
       <c r="H277">
         <v>0.32</v>
@@ -14217,13 +14322,13 @@
     </row>
     <row r="278" spans="1:11">
       <c r="A278" t="s">
-        <v>1084</v>
+        <v>1100</v>
       </c>
       <c r="B278" t="s">
-        <v>1085</v>
+        <v>1101</v>
       </c>
       <c r="C278" t="s">
-        <v>1086</v>
+        <v>1102</v>
       </c>
       <c r="D278">
         <v>0</v>
@@ -14235,7 +14340,7 @@
         <v>0.98151497216733619</v>
       </c>
       <c r="G278" t="s">
-        <v>1087</v>
+        <v>1103</v>
       </c>
       <c r="H278">
         <v>0.88</v>
@@ -14244,7 +14349,7 @@
         <v>0.9456</v>
       </c>
       <c r="J278" t="s">
-        <v>1088</v>
+        <v>1104</v>
       </c>
       <c r="K278">
         <v>0</v>
@@ -14252,13 +14357,13 @@
     </row>
     <row r="279" spans="1:11">
       <c r="A279" t="s">
-        <v>1089</v>
+        <v>1105</v>
       </c>
       <c r="B279" t="s">
-        <v>1090</v>
+        <v>1106</v>
       </c>
       <c r="C279" t="s">
-        <v>1091</v>
+        <v>1107</v>
       </c>
       <c r="D279">
         <v>0</v>
@@ -14270,7 +14375,7 @@
         <v>0.71942500020697597</v>
       </c>
       <c r="G279" t="s">
-        <v>1092</v>
+        <v>1108</v>
       </c>
       <c r="H279">
         <v>0.64</v>
@@ -14279,7 +14384,7 @@
         <v>0.93290000000000006</v>
       </c>
       <c r="J279" t="s">
-        <v>1093</v>
+        <v>1109</v>
       </c>
       <c r="K279">
         <v>0</v>
@@ -14287,13 +14392,13 @@
     </row>
     <row r="280" spans="1:11">
       <c r="A280" t="s">
-        <v>1094</v>
+        <v>1110</v>
       </c>
       <c r="B280" t="s">
-        <v>1095</v>
+        <v>1111</v>
       </c>
       <c r="C280" t="s">
-        <v>1096</v>
+        <v>1112</v>
       </c>
       <c r="D280">
         <v>0</v>
@@ -14305,7 +14410,7 @@
         <v>0.91697247706422014</v>
       </c>
       <c r="G280" t="s">
-        <v>1097</v>
+        <v>1113</v>
       </c>
       <c r="H280">
         <v>0.8</v>
@@ -14314,7 +14419,7 @@
         <v>0.95420000000000005</v>
       </c>
       <c r="J280" t="s">
-        <v>1098</v>
+        <v>1114</v>
       </c>
       <c r="K280">
         <v>0</v>
@@ -14322,13 +14427,13 @@
     </row>
     <row r="281" spans="1:11">
       <c r="A281" t="s">
-        <v>1099</v>
+        <v>1115</v>
       </c>
       <c r="B281" t="s">
-        <v>1100</v>
+        <v>1116</v>
       </c>
       <c r="C281" t="s">
-        <v>1101</v>
+        <v>1117</v>
       </c>
       <c r="D281">
         <v>0</v>
@@ -14340,7 +14445,7 @@
         <v>0.95888877000712913</v>
       </c>
       <c r="G281" t="s">
-        <v>1102</v>
+        <v>1118</v>
       </c>
       <c r="H281">
         <v>0.94</v>
@@ -14349,7 +14454,7 @@
         <v>0.97930000000000006</v>
       </c>
       <c r="J281" t="s">
-        <v>1103</v>
+        <v>1119</v>
       </c>
       <c r="K281">
         <v>0</v>
@@ -14357,13 +14462,13 @@
     </row>
     <row r="282" spans="1:11">
       <c r="A282" t="s">
-        <v>1104</v>
+        <v>1120</v>
       </c>
       <c r="B282" t="s">
-        <v>1105</v>
+        <v>1121</v>
       </c>
       <c r="C282" t="s">
-        <v>1106</v>
+        <v>1122</v>
       </c>
       <c r="D282">
         <v>0</v>
@@ -14375,7 +14480,7 @@
         <v>0.7648210692727796</v>
       </c>
       <c r="G282" t="s">
-        <v>1107</v>
+        <v>1123</v>
       </c>
       <c r="H282">
         <v>0.45</v>
@@ -14384,7 +14489,7 @@
         <v>0.79579999999999995</v>
       </c>
       <c r="J282" t="s">
-        <v>1108</v>
+        <v>1124</v>
       </c>
       <c r="K282">
         <v>0</v>
@@ -14392,13 +14497,13 @@
     </row>
     <row r="283" spans="1:11">
       <c r="A283" t="s">
-        <v>1109</v>
+        <v>1125</v>
       </c>
       <c r="B283" t="s">
-        <v>1110</v>
+        <v>1126</v>
       </c>
       <c r="C283" t="s">
-        <v>1111</v>
+        <v>1127</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -14410,7 +14515,7 @@
         <v>0.51308676160337541</v>
       </c>
       <c r="G283" t="s">
-        <v>1112</v>
+        <v>1128</v>
       </c>
       <c r="H283">
         <v>0.24</v>
@@ -14419,7 +14524,7 @@
         <v>0.80349999999999999</v>
       </c>
       <c r="J283" t="s">
-        <v>1113</v>
+        <v>1129</v>
       </c>
       <c r="K283">
         <v>0</v>
@@ -14427,13 +14532,13 @@
     </row>
     <row r="284" spans="1:11">
       <c r="A284" t="s">
-        <v>1114</v>
+        <v>1130</v>
       </c>
       <c r="B284" t="s">
-        <v>1115</v>
+        <v>1131</v>
       </c>
       <c r="C284" t="s">
-        <v>1116</v>
+        <v>1132</v>
       </c>
       <c r="D284">
         <v>0</v>
@@ -14445,7 +14550,7 @@
         <v>0.7903310628307747</v>
       </c>
       <c r="G284" t="s">
-        <v>1117</v>
+        <v>1133</v>
       </c>
       <c r="H284">
         <v>0.63</v>
@@ -14454,7 +14559,7 @@
         <v>0.87690000000000001</v>
       </c>
       <c r="J284" t="s">
-        <v>1118</v>
+        <v>1134</v>
       </c>
       <c r="K284">
         <v>0</v>
@@ -14462,13 +14567,13 @@
     </row>
     <row r="285" spans="1:11">
       <c r="A285" t="s">
-        <v>1119</v>
+        <v>1135</v>
       </c>
       <c r="B285" t="s">
-        <v>1120</v>
+        <v>1136</v>
       </c>
       <c r="C285" t="s">
-        <v>1121</v>
+        <v>1137</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -14497,13 +14602,13 @@
     </row>
     <row r="286" spans="1:11">
       <c r="A286" t="s">
-        <v>1122</v>
+        <v>1138</v>
       </c>
       <c r="B286" t="s">
-        <v>1123</v>
+        <v>1139</v>
       </c>
       <c r="C286" t="s">
-        <v>1124</v>
+        <v>1140</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -14524,7 +14629,7 @@
         <v>0.92989999999999995</v>
       </c>
       <c r="J286" t="s">
-        <v>1125</v>
+        <v>1141</v>
       </c>
       <c r="K286">
         <v>0</v>
@@ -14532,13 +14637,13 @@
     </row>
     <row r="287" spans="1:11">
       <c r="A287" t="s">
-        <v>1126</v>
+        <v>1142</v>
       </c>
       <c r="B287" t="s">
-        <v>1127</v>
+        <v>1143</v>
       </c>
       <c r="C287" t="s">
-        <v>1128</v>
+        <v>1144</v>
       </c>
       <c r="D287">
         <v>0</v>
@@ -14550,7 +14655,7 @@
         <v>0.99993750000000003</v>
       </c>
       <c r="G287" t="s">
-        <v>1129</v>
+        <v>1145</v>
       </c>
       <c r="H287">
         <v>0.91</v>
@@ -14559,7 +14664,7 @@
         <v>0.98349999999999993</v>
       </c>
       <c r="J287" t="s">
-        <v>1130</v>
+        <v>1146</v>
       </c>
       <c r="K287">
         <v>0</v>
@@ -14567,13 +14672,13 @@
     </row>
     <row r="288" spans="1:11">
       <c r="A288" t="s">
-        <v>1131</v>
+        <v>1147</v>
       </c>
       <c r="B288" t="s">
-        <v>1132</v>
+        <v>1148</v>
       </c>
       <c r="C288" t="s">
-        <v>1133</v>
+        <v>1149</v>
       </c>
       <c r="D288">
         <v>0</v>
@@ -14585,7 +14690,7 @@
         <v>0.82735042735042752</v>
       </c>
       <c r="G288" t="s">
-        <v>1134</v>
+        <v>1150</v>
       </c>
       <c r="H288">
         <v>0.3</v>
@@ -14594,7 +14699,7 @@
         <v>0.63190000000000002</v>
       </c>
       <c r="J288" t="s">
-        <v>1135</v>
+        <v>1151</v>
       </c>
       <c r="K288">
         <v>0</v>
@@ -14602,13 +14707,13 @@
     </row>
     <row r="289" spans="1:11">
       <c r="A289" t="s">
-        <v>1136</v>
+        <v>1152</v>
       </c>
       <c r="B289" t="s">
-        <v>1137</v>
+        <v>1153</v>
       </c>
       <c r="C289" t="s">
-        <v>1138</v>
+        <v>1154</v>
       </c>
       <c r="D289">
         <v>0</v>
@@ -14620,7 +14725,7 @@
         <v>0.97554878048780491</v>
       </c>
       <c r="G289" t="s">
-        <v>1139</v>
+        <v>1155</v>
       </c>
       <c r="H289">
         <v>0.89</v>
@@ -14629,7 +14734,7 @@
         <v>0.96530000000000005</v>
       </c>
       <c r="J289" t="s">
-        <v>1140</v>
+        <v>1156</v>
       </c>
       <c r="K289">
         <v>0</v>
@@ -14637,13 +14742,13 @@
     </row>
     <row r="290" spans="1:11">
       <c r="A290" t="s">
-        <v>1141</v>
+        <v>1157</v>
       </c>
       <c r="B290" t="s">
-        <v>1142</v>
+        <v>1158</v>
       </c>
       <c r="C290" t="s">
-        <v>1143</v>
+        <v>1159</v>
       </c>
       <c r="D290">
         <v>0</v>
@@ -14655,7 +14760,7 @@
         <v>0.9003281771919136</v>
       </c>
       <c r="G290" t="s">
-        <v>1144</v>
+        <v>1160</v>
       </c>
       <c r="H290">
         <v>0.64</v>
@@ -14664,7 +14769,7 @@
         <v>0.8417</v>
       </c>
       <c r="J290" t="s">
-        <v>1145</v>
+        <v>1161</v>
       </c>
       <c r="K290">
         <v>0</v>
@@ -14672,13 +14777,13 @@
     </row>
     <row r="291" spans="1:11">
       <c r="A291" t="s">
-        <v>1146</v>
+        <v>1162</v>
       </c>
       <c r="B291" t="s">
-        <v>1147</v>
+        <v>1163</v>
       </c>
       <c r="C291" t="s">
-        <v>1148</v>
+        <v>1164</v>
       </c>
       <c r="D291">
         <v>0</v>
@@ -14690,7 +14795,7 @@
         <v>0.93197278911564618</v>
       </c>
       <c r="G291" t="s">
-        <v>1149</v>
+        <v>1165</v>
       </c>
       <c r="H291">
         <v>0.69</v>
@@ -14707,13 +14812,13 @@
     </row>
     <row r="292" spans="1:11">
       <c r="A292" t="s">
-        <v>1150</v>
+        <v>1166</v>
       </c>
       <c r="B292" t="s">
-        <v>1151</v>
+        <v>1167</v>
       </c>
       <c r="C292" t="s">
-        <v>1152</v>
+        <v>1168</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -14725,7 +14830,7 @@
         <v>0.65260257994526893</v>
       </c>
       <c r="G292" t="s">
-        <v>1153</v>
+        <v>1169</v>
       </c>
       <c r="H292">
         <v>0.34</v>
@@ -14734,7 +14839,7 @@
         <v>0.74900000000000011</v>
       </c>
       <c r="J292" t="s">
-        <v>1154</v>
+        <v>1170</v>
       </c>
       <c r="K292">
         <v>0</v>
@@ -14742,13 +14847,13 @@
     </row>
     <row r="293" spans="1:11">
       <c r="A293" t="s">
-        <v>1155</v>
+        <v>1171</v>
       </c>
       <c r="B293" t="s">
-        <v>1156</v>
+        <v>1172</v>
       </c>
       <c r="C293" t="s">
-        <v>1157</v>
+        <v>1173</v>
       </c>
       <c r="D293">
         <v>0</v>
@@ -14760,7 +14865,7 @@
         <v>0.91703661742883691</v>
       </c>
       <c r="G293" t="s">
-        <v>1158</v>
+        <v>1174</v>
       </c>
       <c r="H293">
         <v>1</v>
@@ -14769,7 +14874,7 @@
         <v>0.94</v>
       </c>
       <c r="J293" t="s">
-        <v>1159</v>
+        <v>1175</v>
       </c>
       <c r="K293">
         <v>0</v>
@@ -14777,13 +14882,13 @@
     </row>
     <row r="294" spans="1:11">
       <c r="A294" t="s">
-        <v>1160</v>
+        <v>1176</v>
       </c>
       <c r="B294" t="s">
-        <v>1161</v>
+        <v>1177</v>
       </c>
       <c r="C294" t="s">
-        <v>1162</v>
+        <v>1178</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -14795,7 +14900,7 @@
         <v>0.73776919828678289</v>
       </c>
       <c r="G294" t="s">
-        <v>1163</v>
+        <v>1179</v>
       </c>
       <c r="H294">
         <v>0.62</v>
@@ -14804,7 +14909,7 @@
         <v>0.80400000000000005</v>
       </c>
       <c r="J294" t="s">
-        <v>1164</v>
+        <v>1180</v>
       </c>
       <c r="K294">
         <v>0</v>
@@ -14812,13 +14917,13 @@
     </row>
     <row r="295" spans="1:11">
       <c r="A295" t="s">
-        <v>1165</v>
+        <v>1181</v>
       </c>
       <c r="B295" t="s">
-        <v>1166</v>
+        <v>1182</v>
       </c>
       <c r="C295" t="s">
-        <v>1167</v>
+        <v>1183</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -14830,7 +14935,7 @@
         <v>0.89711883308721962</v>
       </c>
       <c r="G295" t="s">
-        <v>1168</v>
+        <v>1184</v>
       </c>
       <c r="H295">
         <v>0.75</v>
@@ -14839,7 +14944,7 @@
         <v>0.93019999999999992</v>
       </c>
       <c r="J295" t="s">
-        <v>1169</v>
+        <v>1185</v>
       </c>
       <c r="K295">
         <v>0</v>
@@ -14847,13 +14952,13 @@
     </row>
     <row r="296" spans="1:11">
       <c r="A296" t="s">
-        <v>1170</v>
+        <v>1186</v>
       </c>
       <c r="B296" t="s">
-        <v>1171</v>
+        <v>1187</v>
       </c>
       <c r="C296" t="s">
-        <v>1172</v>
+        <v>1188</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -14865,7 +14970,7 @@
         <v>0.79250589368334379</v>
       </c>
       <c r="G296" t="s">
-        <v>1173</v>
+        <v>1189</v>
       </c>
       <c r="H296">
         <v>0.71</v>
@@ -14874,7 +14979,7 @@
         <v>0.91689999999999994</v>
       </c>
       <c r="J296" t="s">
-        <v>1174</v>
+        <v>1190</v>
       </c>
       <c r="K296">
         <v>0</v>
@@ -14882,13 +14987,13 @@
     </row>
     <row r="297" spans="1:11">
       <c r="A297" t="s">
-        <v>1175</v>
+        <v>1191</v>
       </c>
       <c r="B297" t="s">
-        <v>1176</v>
+        <v>1192</v>
       </c>
       <c r="C297" t="s">
-        <v>1176</v>
+        <v>1192</v>
       </c>
       <c r="D297">
         <v>1</v>
@@ -14917,13 +15022,13 @@
     </row>
     <row r="298" spans="1:11">
       <c r="A298" t="s">
-        <v>1177</v>
+        <v>1193</v>
       </c>
       <c r="B298" t="s">
-        <v>1178</v>
+        <v>1194</v>
       </c>
       <c r="C298" t="s">
-        <v>1179</v>
+        <v>1195</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -14935,7 +15040,7 @@
         <v>0.99735703251328245</v>
       </c>
       <c r="G298" t="s">
-        <v>1180</v>
+        <v>1196</v>
       </c>
       <c r="H298">
         <v>0.9</v>
@@ -14944,7 +15049,7 @@
         <v>0.95909999999999995</v>
       </c>
       <c r="J298" t="s">
-        <v>1181</v>
+        <v>1197</v>
       </c>
       <c r="K298">
         <v>0</v>
@@ -14952,13 +15057,13 @@
     </row>
     <row r="299" spans="1:11">
       <c r="A299" t="s">
-        <v>1182</v>
+        <v>1198</v>
       </c>
       <c r="B299" t="s">
-        <v>1183</v>
+        <v>1199</v>
       </c>
       <c r="C299" t="s">
-        <v>1184</v>
+        <v>1200</v>
       </c>
       <c r="D299">
         <v>0</v>
@@ -14970,7 +15075,7 @@
         <v>0.85687569193583235</v>
       </c>
       <c r="G299" t="s">
-        <v>1185</v>
+        <v>1201</v>
       </c>
       <c r="H299">
         <v>0.79</v>
@@ -14979,7 +15084,7 @@
         <v>0.98640000000000005</v>
       </c>
       <c r="J299" t="s">
-        <v>1186</v>
+        <v>1202</v>
       </c>
       <c r="K299">
         <v>0</v>
@@ -14987,13 +15092,13 @@
     </row>
     <row r="300" spans="1:11">
       <c r="A300" t="s">
-        <v>1187</v>
+        <v>1203</v>
       </c>
       <c r="B300" t="s">
-        <v>1188</v>
+        <v>1204</v>
       </c>
       <c r="C300" t="s">
-        <v>1189</v>
+        <v>1205</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -15005,7 +15110,7 @@
         <v>0.86221105326895342</v>
       </c>
       <c r="G300" t="s">
-        <v>1190</v>
+        <v>1206</v>
       </c>
       <c r="H300">
         <v>0.71</v>
@@ -15014,7 +15119,7 @@
         <v>0.93730000000000002</v>
       </c>
       <c r="J300" t="s">
-        <v>1191</v>
+        <v>1207</v>
       </c>
       <c r="K300">
         <v>0</v>
@@ -15022,13 +15127,13 @@
     </row>
     <row r="301" spans="1:11">
       <c r="A301" t="s">
-        <v>1192</v>
+        <v>1208</v>
       </c>
       <c r="B301" t="s">
-        <v>1193</v>
+        <v>1209</v>
       </c>
       <c r="C301" t="s">
-        <v>1194</v>
+        <v>1210</v>
       </c>
       <c r="D301">
         <v>0</v>
@@ -15040,7 +15145,7 @@
         <v>0.99610749193911696</v>
       </c>
       <c r="G301" t="s">
-        <v>1195</v>
+        <v>1211</v>
       </c>
       <c r="H301">
         <v>0.85</v>
@@ -15049,7 +15154,7 @@
         <v>0.96879999999999999</v>
       </c>
       <c r="J301" t="s">
-        <v>1196</v>
+        <v>1212</v>
       </c>
       <c r="K301">
         <v>0</v>
@@ -15057,13 +15162,13 @@
     </row>
     <row r="302" spans="1:11">
       <c r="A302" t="s">
-        <v>1197</v>
+        <v>1213</v>
       </c>
       <c r="B302" t="s">
-        <v>1198</v>
+        <v>1214</v>
       </c>
       <c r="C302" t="s">
-        <v>1199</v>
+        <v>1215</v>
       </c>
       <c r="D302">
         <v>0</v>
@@ -15075,7 +15180,7 @@
         <v>0.78805201069249298</v>
       </c>
       <c r="G302" t="s">
-        <v>1200</v>
+        <v>1216</v>
       </c>
       <c r="H302">
         <v>0.7</v>
@@ -15084,7 +15189,7 @@
         <v>0.93129999999999991</v>
       </c>
       <c r="J302" t="s">
-        <v>1201</v>
+        <v>1217</v>
       </c>
       <c r="K302">
         <v>0</v>
@@ -15092,13 +15197,13 @@
     </row>
     <row r="303" spans="1:11">
       <c r="A303" t="s">
-        <v>1202</v>
+        <v>1218</v>
       </c>
       <c r="B303" t="s">
-        <v>1203</v>
+        <v>1219</v>
       </c>
       <c r="C303" t="s">
-        <v>1204</v>
+        <v>1220</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -15110,7 +15215,7 @@
         <v>0.96943863981762923</v>
       </c>
       <c r="G303" t="s">
-        <v>1205</v>
+        <v>1221</v>
       </c>
       <c r="H303">
         <v>0.39</v>
@@ -15119,7 +15224,7 @@
         <v>0.8</v>
       </c>
       <c r="J303" t="s">
-        <v>1206</v>
+        <v>1222</v>
       </c>
       <c r="K303">
         <v>0</v>
@@ -15127,13 +15232,13 @@
     </row>
     <row r="304" spans="1:11">
       <c r="A304" t="s">
-        <v>1207</v>
+        <v>1223</v>
       </c>
       <c r="B304" t="s">
-        <v>1208</v>
+        <v>1224</v>
       </c>
       <c r="C304" t="s">
-        <v>1209</v>
+        <v>1225</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -15145,7 +15250,7 @@
         <v>0.93118385612182153</v>
       </c>
       <c r="G304" t="s">
-        <v>1210</v>
+        <v>1226</v>
       </c>
       <c r="H304">
         <v>1</v>
@@ -15154,7 +15259,7 @@
         <v>0.97329999999999994</v>
       </c>
       <c r="J304" t="s">
-        <v>1211</v>
+        <v>1227</v>
       </c>
       <c r="K304">
         <v>0</v>
@@ -15162,13 +15267,13 @@
     </row>
     <row r="305" spans="1:11">
       <c r="A305" t="s">
-        <v>1212</v>
+        <v>1228</v>
       </c>
       <c r="B305" t="s">
-        <v>1213</v>
+        <v>1229</v>
       </c>
       <c r="C305" t="s">
-        <v>1214</v>
+        <v>1230</v>
       </c>
       <c r="D305">
         <v>0</v>
@@ -15180,7 +15285,7 @@
         <v>0.92150987268919982</v>
       </c>
       <c r="G305" t="s">
-        <v>1215</v>
+        <v>1231</v>
       </c>
       <c r="H305">
         <v>0.73</v>
@@ -15189,7 +15294,7 @@
         <v>0.86599999999999999</v>
       </c>
       <c r="J305" t="s">
-        <v>1216</v>
+        <v>1232</v>
       </c>
       <c r="K305">
         <v>0</v>
@@ -15197,13 +15302,13 @@
     </row>
     <row r="306" spans="1:11">
       <c r="A306" t="s">
-        <v>1217</v>
+        <v>1233</v>
       </c>
       <c r="B306" t="s">
-        <v>1218</v>
+        <v>1234</v>
       </c>
       <c r="C306" t="s">
-        <v>1218</v>
+        <v>1234</v>
       </c>
       <c r="D306">
         <v>1</v>
@@ -15232,13 +15337,13 @@
     </row>
     <row r="307" spans="1:11">
       <c r="A307" t="s">
-        <v>1219</v>
+        <v>1235</v>
       </c>
       <c r="B307" t="s">
-        <v>1220</v>
+        <v>1236</v>
       </c>
       <c r="C307" t="s">
-        <v>1221</v>
+        <v>1237</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -15250,7 +15355,7 @@
         <v>0.84459459459459441</v>
       </c>
       <c r="G307" t="s">
-        <v>1222</v>
+        <v>1238</v>
       </c>
       <c r="H307">
         <v>0.62</v>
@@ -15259,7 +15364,7 @@
         <v>0.95609999999999995</v>
       </c>
       <c r="J307" t="s">
-        <v>1223</v>
+        <v>1239</v>
       </c>
       <c r="K307">
         <v>0</v>
@@ -15267,13 +15372,13 @@
     </row>
     <row r="308" spans="1:11">
       <c r="A308" t="s">
-        <v>1224</v>
+        <v>1240</v>
       </c>
       <c r="B308" t="s">
-        <v>1225</v>
+        <v>1241</v>
       </c>
       <c r="C308" t="s">
-        <v>1226</v>
+        <v>1242</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -15285,7 +15390,7 @@
         <v>0.88969017094017089</v>
       </c>
       <c r="G308" t="s">
-        <v>1227</v>
+        <v>1243</v>
       </c>
       <c r="H308">
         <v>0.52</v>
@@ -15294,7 +15399,7 @@
         <v>0.79569999999999996</v>
       </c>
       <c r="J308" t="s">
-        <v>1228</v>
+        <v>1244</v>
       </c>
       <c r="K308">
         <v>0</v>
@@ -15302,13 +15407,13 @@
     </row>
     <row r="309" spans="1:11">
       <c r="A309" t="s">
-        <v>1229</v>
+        <v>1245</v>
       </c>
       <c r="B309" t="s">
-        <v>1230</v>
+        <v>1246</v>
       </c>
       <c r="C309" t="s">
-        <v>1231</v>
+        <v>1247</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -15320,7 +15425,7 @@
         <v>0.91395863315515335</v>
       </c>
       <c r="G309" t="s">
-        <v>1232</v>
+        <v>1248</v>
       </c>
       <c r="H309">
         <v>0.71</v>
@@ -15329,7 +15434,7 @@
         <v>0.9173</v>
       </c>
       <c r="J309" t="s">
-        <v>1233</v>
+        <v>1249</v>
       </c>
       <c r="K309">
         <v>0</v>
@@ -15337,13 +15442,13 @@
     </row>
     <row r="310" spans="1:11">
       <c r="A310" t="s">
-        <v>1234</v>
+        <v>1250</v>
       </c>
       <c r="B310" t="s">
-        <v>1235</v>
+        <v>1251</v>
       </c>
       <c r="C310" t="s">
-        <v>1235</v>
+        <v>1251</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -15372,13 +15477,13 @@
     </row>
     <row r="311" spans="1:11">
       <c r="A311" t="s">
-        <v>1236</v>
+        <v>1252</v>
       </c>
       <c r="B311" t="s">
-        <v>1237</v>
+        <v>1253</v>
       </c>
       <c r="C311" t="s">
-        <v>1238</v>
+        <v>1254</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -15390,7 +15495,7 @@
         <v>0.58455728246307592</v>
       </c>
       <c r="G311" t="s">
-        <v>1239</v>
+        <v>1255</v>
       </c>
       <c r="H311">
         <v>0.22</v>
@@ -15399,7 +15504,7 @@
         <v>0.86419999999999997</v>
       </c>
       <c r="J311" t="s">
-        <v>1240</v>
+        <v>1256</v>
       </c>
       <c r="K311">
         <v>0</v>
@@ -15407,13 +15512,13 @@
     </row>
     <row r="312" spans="1:11">
       <c r="A312" t="s">
-        <v>1241</v>
+        <v>1257</v>
       </c>
       <c r="B312" t="s">
-        <v>1242</v>
+        <v>1258</v>
       </c>
       <c r="C312" t="s">
-        <v>1243</v>
+        <v>1259</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -15425,7 +15530,7 @@
         <v>0.96341746046674104</v>
       </c>
       <c r="G312" t="s">
-        <v>1244</v>
+        <v>1260</v>
       </c>
       <c r="H312">
         <v>0.82</v>
@@ -15434,7 +15539,7 @@
         <v>0.9375</v>
       </c>
       <c r="J312" t="s">
-        <v>1245</v>
+        <v>1261</v>
       </c>
       <c r="K312">
         <v>0</v>
@@ -15442,13 +15547,13 @@
     </row>
     <row r="313" spans="1:11">
       <c r="A313" t="s">
-        <v>1246</v>
+        <v>1262</v>
       </c>
       <c r="B313" t="s">
-        <v>1247</v>
+        <v>1263</v>
       </c>
       <c r="C313" t="s">
-        <v>1248</v>
+        <v>1264</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -15460,7 +15565,7 @@
         <v>0.78049017672603971</v>
       </c>
       <c r="G313" t="s">
-        <v>1249</v>
+        <v>1265</v>
       </c>
       <c r="H313">
         <v>0.84</v>
@@ -15469,7 +15574,7 @@
         <v>0.94830000000000003</v>
       </c>
       <c r="J313" t="s">
-        <v>1250</v>
+        <v>1266</v>
       </c>
       <c r="K313">
         <v>0</v>
@@ -15477,13 +15582,13 @@
     </row>
     <row r="314" spans="1:11">
       <c r="A314" t="s">
-        <v>1251</v>
+        <v>1267</v>
       </c>
       <c r="B314" t="s">
-        <v>1252</v>
+        <v>1268</v>
       </c>
       <c r="C314" t="s">
-        <v>1253</v>
+        <v>1269</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -15495,7 +15600,7 @@
         <v>0.90394202898550713</v>
       </c>
       <c r="G314" t="s">
-        <v>1254</v>
+        <v>1270</v>
       </c>
       <c r="H314">
         <v>0.92</v>
@@ -15504,7 +15609,7 @@
         <v>0.96870000000000001</v>
       </c>
       <c r="J314" t="s">
-        <v>1255</v>
+        <v>1271</v>
       </c>
       <c r="K314">
         <v>0</v>
@@ -15512,13 +15617,13 @@
     </row>
     <row r="315" spans="1:11">
       <c r="A315" t="s">
-        <v>1256</v>
+        <v>1272</v>
       </c>
       <c r="B315" t="s">
-        <v>1257</v>
+        <v>1273</v>
       </c>
       <c r="C315" t="s">
-        <v>1258</v>
+        <v>1274</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -15530,7 +15635,7 @@
         <v>0.87517556179775269</v>
       </c>
       <c r="G315" t="s">
-        <v>1259</v>
+        <v>1275</v>
       </c>
       <c r="H315">
         <v>0.5</v>
@@ -15547,13 +15652,13 @@
     </row>
     <row r="316" spans="1:11">
       <c r="A316" t="s">
-        <v>1260</v>
+        <v>1276</v>
       </c>
       <c r="B316" t="s">
-        <v>1261</v>
+        <v>1277</v>
       </c>
       <c r="C316" t="s">
-        <v>1262</v>
+        <v>1278</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -15565,7 +15670,7 @@
         <v>0.77401692384270782</v>
       </c>
       <c r="G316" t="s">
-        <v>1263</v>
+        <v>1279</v>
       </c>
       <c r="H316">
         <v>0.49</v>
@@ -15574,7 +15679,7 @@
         <v>0.88280000000000003</v>
       </c>
       <c r="J316" t="s">
-        <v>1264</v>
+        <v>1280</v>
       </c>
       <c r="K316">
         <v>0</v>
@@ -15582,13 +15687,13 @@
     </row>
     <row r="317" spans="1:11">
       <c r="A317" t="s">
-        <v>1265</v>
+        <v>1281</v>
       </c>
       <c r="B317" t="s">
-        <v>1266</v>
+        <v>1282</v>
       </c>
       <c r="C317" t="s">
-        <v>1267</v>
+        <v>1283</v>
       </c>
       <c r="D317">
         <v>0</v>
@@ -15600,7 +15705,7 @@
         <v>0.70448824816204658</v>
       </c>
       <c r="G317" t="s">
-        <v>1268</v>
+        <v>1284</v>
       </c>
       <c r="H317">
         <v>0.53</v>
@@ -15609,7 +15714,7 @@
         <v>0.9103</v>
       </c>
       <c r="J317" t="s">
-        <v>1269</v>
+        <v>1285</v>
       </c>
       <c r="K317">
         <v>0</v>
@@ -15617,13 +15722,13 @@
     </row>
     <row r="318" spans="1:11">
       <c r="A318" t="s">
-        <v>1270</v>
+        <v>1286</v>
       </c>
       <c r="B318" t="s">
-        <v>1271</v>
+        <v>1287</v>
       </c>
       <c r="C318" t="s">
-        <v>1272</v>
+        <v>1288</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -15635,7 +15740,7 @@
         <v>0.8578868267449582</v>
       </c>
       <c r="G318" t="s">
-        <v>1273</v>
+        <v>1289</v>
       </c>
       <c r="H318">
         <v>1</v>
@@ -15644,7 +15749,7 @@
         <v>0.93700000000000006</v>
       </c>
       <c r="J318" t="s">
-        <v>1274</v>
+        <v>1290</v>
       </c>
       <c r="K318">
         <v>0</v>
@@ -15652,13 +15757,13 @@
     </row>
     <row r="319" spans="1:11">
       <c r="A319" t="s">
-        <v>1275</v>
+        <v>1291</v>
       </c>
       <c r="B319" t="s">
-        <v>1276</v>
+        <v>1292</v>
       </c>
       <c r="C319" t="s">
-        <v>1277</v>
+        <v>1293</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -15670,7 +15775,7 @@
         <v>0.98576950809165209</v>
       </c>
       <c r="G319" t="s">
-        <v>1278</v>
+        <v>1294</v>
       </c>
       <c r="H319">
         <v>0.91</v>
@@ -15679,7 +15784,7 @@
         <v>0.96109999999999995</v>
       </c>
       <c r="J319" t="s">
-        <v>1279</v>
+        <v>1295</v>
       </c>
       <c r="K319">
         <v>0</v>
@@ -15687,13 +15792,13 @@
     </row>
     <row r="320" spans="1:11">
       <c r="A320" t="s">
-        <v>1280</v>
+        <v>1296</v>
       </c>
       <c r="B320" t="s">
-        <v>1281</v>
+        <v>1297</v>
       </c>
       <c r="C320" t="s">
-        <v>1282</v>
+        <v>1298</v>
       </c>
       <c r="D320">
         <v>0</v>
@@ -15705,7 +15810,7 @@
         <v>0.99142030393168623</v>
       </c>
       <c r="G320" t="s">
-        <v>1283</v>
+        <v>1299</v>
       </c>
       <c r="H320">
         <v>0.84</v>
@@ -15722,13 +15827,13 @@
     </row>
     <row r="321" spans="1:11">
       <c r="A321" t="s">
-        <v>1284</v>
+        <v>1300</v>
       </c>
       <c r="B321" t="s">
-        <v>1285</v>
+        <v>1301</v>
       </c>
       <c r="C321" t="s">
-        <v>1285</v>
+        <v>1301</v>
       </c>
       <c r="D321">
         <v>1</v>
@@ -15757,13 +15862,13 @@
     </row>
     <row r="322" spans="1:11">
       <c r="A322" t="s">
-        <v>1286</v>
+        <v>1302</v>
       </c>
       <c r="B322" t="s">
-        <v>1287</v>
+        <v>1303</v>
       </c>
       <c r="C322" t="s">
-        <v>1288</v>
+        <v>1304</v>
       </c>
       <c r="D322">
         <v>0</v>
@@ -15775,7 +15880,7 @@
         <v>0.95990232827825017</v>
       </c>
       <c r="G322" t="s">
-        <v>1289</v>
+        <v>1305</v>
       </c>
       <c r="H322">
         <v>0.59</v>
@@ -15784,7 +15889,7 @@
         <v>0.8427</v>
       </c>
       <c r="J322" t="s">
-        <v>1290</v>
+        <v>1306</v>
       </c>
       <c r="K322">
         <v>0</v>
@@ -15792,13 +15897,13 @@
     </row>
     <row r="323" spans="1:11">
       <c r="A323" t="s">
-        <v>1291</v>
+        <v>1307</v>
       </c>
       <c r="B323" t="s">
-        <v>1292</v>
+        <v>1308</v>
       </c>
       <c r="C323" t="s">
-        <v>1293</v>
+        <v>1309</v>
       </c>
       <c r="D323">
         <v>0</v>
@@ -15810,7 +15915,7 @@
         <v>0.91487850396871861</v>
       </c>
       <c r="G323" t="s">
-        <v>1294</v>
+        <v>1310</v>
       </c>
       <c r="H323">
         <v>0.88</v>
@@ -15819,7 +15924,7 @@
         <v>0.95950000000000002</v>
       </c>
       <c r="J323" t="s">
-        <v>1295</v>
+        <v>1311</v>
       </c>
       <c r="K323">
         <v>0</v>
@@ -15827,13 +15932,13 @@
     </row>
     <row r="324" spans="1:11">
       <c r="A324" t="s">
-        <v>1296</v>
+        <v>1312</v>
       </c>
       <c r="B324" t="s">
-        <v>1297</v>
+        <v>1313</v>
       </c>
       <c r="C324" t="s">
-        <v>1298</v>
+        <v>1314</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -15845,7 +15950,7 @@
         <v>0.84168421052631581</v>
       </c>
       <c r="G324" t="s">
-        <v>1299</v>
+        <v>1315</v>
       </c>
       <c r="H324">
         <v>0.62</v>
@@ -15854,7 +15959,7 @@
         <v>0.92590000000000006</v>
       </c>
       <c r="J324" t="s">
-        <v>1245</v>
+        <v>1261</v>
       </c>
       <c r="K324">
         <v>0</v>
@@ -15862,13 +15967,13 @@
     </row>
     <row r="325" spans="1:11">
       <c r="A325" t="s">
-        <v>1300</v>
+        <v>1316</v>
       </c>
       <c r="B325" t="s">
-        <v>1301</v>
+        <v>1317</v>
       </c>
       <c r="C325" t="s">
-        <v>1302</v>
+        <v>1318</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -15880,7 +15985,7 @@
         <v>0.89947226617328602</v>
       </c>
       <c r="G325" t="s">
-        <v>1303</v>
+        <v>1319</v>
       </c>
       <c r="H325">
         <v>0.74</v>
@@ -15889,7 +15994,7 @@
         <v>0.93849999999999989</v>
       </c>
       <c r="J325" t="s">
-        <v>1304</v>
+        <v>1320</v>
       </c>
       <c r="K325">
         <v>1</v>
@@ -15897,13 +16002,13 @@
     </row>
     <row r="326" spans="1:11">
       <c r="A326" t="s">
-        <v>1305</v>
+        <v>1321</v>
       </c>
       <c r="B326" t="s">
-        <v>1306</v>
+        <v>1322</v>
       </c>
       <c r="C326" t="s">
-        <v>1307</v>
+        <v>1323</v>
       </c>
       <c r="D326">
         <v>0</v>
@@ -15915,7 +16020,7 @@
         <v>0.98131106566689386</v>
       </c>
       <c r="G326" t="s">
-        <v>1308</v>
+        <v>1324</v>
       </c>
       <c r="H326">
         <v>0.92</v>
@@ -15924,7 +16029,7 @@
         <v>0.98769999999999991</v>
       </c>
       <c r="J326" t="s">
-        <v>1309</v>
+        <v>1325</v>
       </c>
       <c r="K326">
         <v>1</v>
@@ -15932,13 +16037,13 @@
     </row>
     <row r="327" spans="1:11">
       <c r="A327" t="s">
-        <v>1310</v>
+        <v>1326</v>
       </c>
       <c r="B327" t="s">
-        <v>1311</v>
+        <v>1327</v>
       </c>
       <c r="C327" t="s">
-        <v>1312</v>
+        <v>1328</v>
       </c>
       <c r="D327">
         <v>0</v>
@@ -15950,7 +16055,7 @@
         <v>0.78317639673571882</v>
       </c>
       <c r="G327" t="s">
-        <v>1313</v>
+        <v>1329</v>
       </c>
       <c r="H327">
         <v>0.6</v>
@@ -15959,7 +16064,7 @@
         <v>0.7742</v>
       </c>
       <c r="J327" t="s">
-        <v>1314</v>
+        <v>1330</v>
       </c>
       <c r="K327">
         <v>1</v>

</xml_diff>

<commit_message>
Aggiunte nuove analisi di Claude Sonnet e aggiunto report per il prof
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiClaudeSonnet.xlsx
+++ b/HE/W_in_progress/AnalisiClaudeSonnet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D435324F-ABE0-4549-BDA1-53BF2DD82313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{681E22F3-AB23-493F-9BEA-38F3C4F9F21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="1331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="1341">
   <si>
     <t>IN</t>
   </si>
@@ -3126,6 +3126,9 @@
     <t>0.4657534208069057</t>
   </si>
   <si>
+    <t>Effettivamente non mi chiede di inizializzare u entity</t>
+  </si>
+  <si>
     <t>Create a configurable clock divider</t>
   </si>
   <si>
@@ -3156,6 +3159,9 @@
     <t>0.15999999503200013</t>
   </si>
   <si>
+    <t>La definisce solo, non implementa</t>
+  </si>
+  <si>
     <t>Define a barrel shifter of N-bit with the signals data_in (N-bit), shift_left, shift_right, and shift_amount as input and the signal data_out (N-bit) as output.</t>
   </si>
   <si>
@@ -3231,6 +3237,9 @@
     <t>0.7407407358024692</t>
   </si>
   <si>
+    <t>Prevede anche un toggle, ma va bene</t>
+  </si>
+  <si>
     <t>Create a BCD to 7-segment display decoder</t>
   </si>
   <si>
@@ -3246,6 +3255,9 @@
     <t>0.049999995450000424</t>
   </si>
   <si>
+    <t>Va bene, anche se naive</t>
+  </si>
+  <si>
     <t>Generate a single clock pulse using a process.</t>
   </si>
   <si>
@@ -3261,6 +3273,9 @@
     <t>0.12903225369406884</t>
   </si>
   <si>
+    <t>Piccoli problemi, ma va bene nel nostro caso</t>
+  </si>
+  <si>
     <t>Implement a basic UART (Universal Asynchronous Receiver/Transmitter) transmitter</t>
   </si>
   <si>
@@ -3276,6 +3291,9 @@
     <t>0.13333332888888905</t>
   </si>
   <si>
+    <t>Non implementa,definisce solo</t>
+  </si>
+  <si>
     <t>Define a parallel in parallel out shift register of N-bit with the signals clock, load_enable, shift_enable, shift_direction, and data_in (N-bit) as input and the signal data_out (N-bit) as output.</t>
   </si>
   <si>
@@ -3321,6 +3339,9 @@
     <t>0.15384615029585808</t>
   </si>
   <si>
+    <t>La condizione è buona, ma non scrive un comparaore</t>
+  </si>
+  <si>
     <t>core_type is an array of 1024 bits of std_logic_vector of 16 bits; use of real math functions; set req signal to '0' when the current state is ASPETTA and if ack signal is low, set next state to FINITO otherwise set next state to ASPETTA</t>
   </si>
   <si>
@@ -3333,6 +3354,9 @@
     <t>0.620253164556962</t>
   </si>
   <si>
+    <t>Manca una condizione</t>
+  </si>
+  <si>
     <t>on the rising edge of clk_in, if clear_sig signal is high set idx variable to 5, set stop_sig signal to '0', increment the variable idx by three; mux0 is an instance of mux_2_1 component with signal a0 mapped to b0, a1 mapped to b1, s mapped to s0, y mapped to u0</t>
   </si>
   <si>
@@ -3408,6 +3432,9 @@
     <t>0.5641025591058515</t>
   </si>
   <si>
+    <t>Non risponde al un sottoprompt (p_arst is an istance of arst)</t>
+  </si>
+  <si>
     <t>map strobe_i to t_stb; This is a component named FullAdderSub with 4 input std_logic signals C_in, A, B, Add_Sub and 2 output std_logic signals Sum; half_adder is the entity for the half adder</t>
   </si>
   <si>
@@ -3487,6 +3514,9 @@
   </si>
   <si>
     <t>0.5161290272632676</t>
+  </si>
+  <si>
+    <t>Altra cosa proprio</t>
   </si>
   <si>
     <t>COUT_RCA gets assigned the N-1-th element from cout_int; d is a constant of type std_logic_vector of 7 bit initialized to '0100001'; define the signal TbClockB whose state changes after TbPeriodB when TbSimEnded is different from '1', otherwise it is '0'</t>
@@ -4412,8 +4442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C243" workbookViewId="0">
-      <selection activeCell="K261" sqref="K261"/>
+    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
+      <selection activeCell="K291" sqref="K291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13757,7 +13787,7 @@
         <v>1020</v>
       </c>
       <c r="K261">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="262" spans="1:12">
@@ -13792,7 +13822,7 @@
         <v>1025</v>
       </c>
       <c r="K262">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="263" spans="1:12">
@@ -13827,18 +13857,21 @@
         <v>1030</v>
       </c>
       <c r="K263">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L263" t="s">
+        <v>1031</v>
       </c>
     </row>
     <row r="264" spans="1:12">
       <c r="A264" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B264" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="C264" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -13850,7 +13883,7 @@
         <v>0.84416716690964189</v>
       </c>
       <c r="G264" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="H264">
         <v>0.35</v>
@@ -13859,21 +13892,21 @@
         <v>0.90930000000000011</v>
       </c>
       <c r="J264" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="K264">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="265" spans="1:12">
       <c r="A265" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B265" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="C265" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -13885,7 +13918,7 @@
         <v>0.1251506024096386</v>
       </c>
       <c r="G265" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="H265">
         <v>0.06</v>
@@ -13894,21 +13927,24 @@
         <v>0.76980000000000004</v>
       </c>
       <c r="J265" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="K265">
         <v>0</v>
+      </c>
+      <c r="L265" t="s">
+        <v>1042</v>
       </c>
     </row>
     <row r="266" spans="1:12">
       <c r="A266" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="B266" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="C266" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -13920,7 +13956,7 @@
         <v>0.37008194888083268</v>
       </c>
       <c r="G266" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="H266">
         <v>0</v>
@@ -13929,21 +13965,21 @@
         <v>0.63029999999999997</v>
       </c>
       <c r="J266" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="K266">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267" spans="1:12">
       <c r="A267" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="B267" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="C267" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -13955,7 +13991,7 @@
         <v>0.34369246118287677</v>
       </c>
       <c r="G267" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="H267">
         <v>0</v>
@@ -13964,21 +14000,21 @@
         <v>0.75950000000000006</v>
       </c>
       <c r="J267" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="K267">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268" spans="1:12">
       <c r="A268" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="B268" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="C268" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -13990,7 +14026,7 @@
         <v>0.39675422756399409</v>
       </c>
       <c r="G268" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="H268">
         <v>0.02</v>
@@ -13999,21 +14035,21 @@
         <v>0.77049999999999996</v>
       </c>
       <c r="J268" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="K268">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269" spans="1:12">
       <c r="A269" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="B269" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="C269" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -14025,7 +14061,7 @@
         <v>0.51819301340860968</v>
       </c>
       <c r="G269" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="H269">
         <v>0.33</v>
@@ -14034,21 +14070,21 @@
         <v>0.75029999999999997</v>
       </c>
       <c r="J269" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="K269">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270" spans="1:12">
       <c r="A270" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="B270" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="C270" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -14060,7 +14096,7 @@
         <v>0.9534105229993699</v>
       </c>
       <c r="G270" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="H270">
         <v>0</v>
@@ -14069,21 +14105,24 @@
         <v>0.77689999999999992</v>
       </c>
       <c r="J270" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="K270">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L270" t="s">
+        <v>1068</v>
       </c>
     </row>
     <row r="271" spans="1:12">
       <c r="A271" t="s">
-        <v>1066</v>
+        <v>1069</v>
       </c>
       <c r="B271" t="s">
-        <v>1067</v>
+        <v>1070</v>
       </c>
       <c r="C271" t="s">
-        <v>1068</v>
+        <v>1071</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -14095,7 +14134,7 @@
         <v>0.24438254450451111</v>
       </c>
       <c r="G271" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
       <c r="H271">
         <v>0.02</v>
@@ -14104,21 +14143,24 @@
         <v>0.47339999999999999</v>
       </c>
       <c r="J271" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
       <c r="K271">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L271" t="s">
+        <v>1074</v>
       </c>
     </row>
     <row r="272" spans="1:12">
       <c r="A272" t="s">
-        <v>1071</v>
+        <v>1075</v>
       </c>
       <c r="B272" t="s">
-        <v>1072</v>
+        <v>1076</v>
       </c>
       <c r="C272" t="s">
-        <v>1073</v>
+        <v>1077</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -14130,7 +14172,7 @@
         <v>0.64418346204022925</v>
       </c>
       <c r="G272" t="s">
-        <v>1074</v>
+        <v>1078</v>
       </c>
       <c r="H272">
         <v>0.31</v>
@@ -14139,21 +14181,24 @@
         <v>0.8909999999999999</v>
       </c>
       <c r="J272" t="s">
-        <v>1075</v>
+        <v>1079</v>
       </c>
       <c r="K272">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L272" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12">
       <c r="A273" t="s">
-        <v>1076</v>
+        <v>1081</v>
       </c>
       <c r="B273" t="s">
-        <v>1077</v>
+        <v>1082</v>
       </c>
       <c r="C273" t="s">
-        <v>1078</v>
+        <v>1083</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -14165,7 +14210,7 @@
         <v>6.5000763591936475E-2</v>
       </c>
       <c r="G273" t="s">
-        <v>1079</v>
+        <v>1084</v>
       </c>
       <c r="H273">
         <v>0</v>
@@ -14174,21 +14219,24 @@
         <v>0.74400000000000011</v>
       </c>
       <c r="J273" t="s">
-        <v>1080</v>
+        <v>1085</v>
       </c>
       <c r="K273">
         <v>0</v>
       </c>
-    </row>
-    <row r="274" spans="1:11">
+      <c r="L273" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12">
       <c r="A274" t="s">
-        <v>1081</v>
+        <v>1087</v>
       </c>
       <c r="B274" t="s">
-        <v>1082</v>
+        <v>1088</v>
       </c>
       <c r="C274" t="s">
-        <v>1083</v>
+        <v>1089</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -14200,7 +14248,7 @@
         <v>0.33160074536381162</v>
       </c>
       <c r="G274" t="s">
-        <v>1084</v>
+        <v>1090</v>
       </c>
       <c r="H274">
         <v>0</v>
@@ -14209,21 +14257,21 @@
         <v>0.76439999999999997</v>
       </c>
       <c r="J274" t="s">
-        <v>1085</v>
+        <v>1091</v>
       </c>
       <c r="K274">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12">
       <c r="A275" t="s">
-        <v>1086</v>
+        <v>1092</v>
       </c>
       <c r="B275" t="s">
-        <v>1087</v>
+        <v>1093</v>
       </c>
       <c r="C275" t="s">
-        <v>1088</v>
+        <v>1094</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -14235,7 +14283,7 @@
         <v>0.36656284712390819</v>
       </c>
       <c r="G275" t="s">
-        <v>1089</v>
+        <v>1095</v>
       </c>
       <c r="H275">
         <v>0</v>
@@ -14244,21 +14292,21 @@
         <v>0.77849999999999997</v>
       </c>
       <c r="J275" t="s">
-        <v>1090</v>
+        <v>1096</v>
       </c>
       <c r="K275">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12">
       <c r="A276" t="s">
-        <v>1091</v>
+        <v>1097</v>
       </c>
       <c r="B276" t="s">
-        <v>1092</v>
+        <v>1098</v>
       </c>
       <c r="C276" t="s">
-        <v>1093</v>
+        <v>1099</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -14270,7 +14318,7 @@
         <v>0.26366390187782968</v>
       </c>
       <c r="G276" t="s">
-        <v>1094</v>
+        <v>1100</v>
       </c>
       <c r="H276">
         <v>0</v>
@@ -14279,21 +14327,24 @@
         <v>0.22750000000000001</v>
       </c>
       <c r="J276" t="s">
-        <v>1095</v>
+        <v>1101</v>
       </c>
       <c r="K276">
         <v>0</v>
       </c>
-    </row>
-    <row r="277" spans="1:11">
+      <c r="L276" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12">
       <c r="A277" t="s">
-        <v>1096</v>
+        <v>1103</v>
       </c>
       <c r="B277" t="s">
-        <v>1097</v>
+        <v>1104</v>
       </c>
       <c r="C277" t="s">
-        <v>1098</v>
+        <v>1105</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -14305,7 +14356,7 @@
         <v>0.54521926556252653</v>
       </c>
       <c r="G277" t="s">
-        <v>1099</v>
+        <v>1106</v>
       </c>
       <c r="H277">
         <v>0.32</v>
@@ -14319,16 +14370,19 @@
       <c r="K277">
         <v>0</v>
       </c>
-    </row>
-    <row r="278" spans="1:11">
+      <c r="L277" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12">
       <c r="A278" t="s">
-        <v>1100</v>
+        <v>1108</v>
       </c>
       <c r="B278" t="s">
-        <v>1101</v>
+        <v>1109</v>
       </c>
       <c r="C278" t="s">
-        <v>1102</v>
+        <v>1110</v>
       </c>
       <c r="D278">
         <v>0</v>
@@ -14340,7 +14394,7 @@
         <v>0.98151497216733619</v>
       </c>
       <c r="G278" t="s">
-        <v>1103</v>
+        <v>1111</v>
       </c>
       <c r="H278">
         <v>0.88</v>
@@ -14349,21 +14403,24 @@
         <v>0.9456</v>
       </c>
       <c r="J278" t="s">
-        <v>1104</v>
+        <v>1112</v>
       </c>
       <c r="K278">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="279" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L278" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12">
       <c r="A279" t="s">
-        <v>1105</v>
+        <v>1113</v>
       </c>
       <c r="B279" t="s">
-        <v>1106</v>
+        <v>1114</v>
       </c>
       <c r="C279" t="s">
-        <v>1107</v>
+        <v>1115</v>
       </c>
       <c r="D279">
         <v>0</v>
@@ -14375,7 +14432,7 @@
         <v>0.71942500020697597</v>
       </c>
       <c r="G279" t="s">
-        <v>1108</v>
+        <v>1116</v>
       </c>
       <c r="H279">
         <v>0.64</v>
@@ -14384,21 +14441,21 @@
         <v>0.93290000000000006</v>
       </c>
       <c r="J279" t="s">
-        <v>1109</v>
+        <v>1117</v>
       </c>
       <c r="K279">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="280" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12">
       <c r="A280" t="s">
-        <v>1110</v>
+        <v>1118</v>
       </c>
       <c r="B280" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="C280" t="s">
-        <v>1112</v>
+        <v>1120</v>
       </c>
       <c r="D280">
         <v>0</v>
@@ -14410,7 +14467,7 @@
         <v>0.91697247706422014</v>
       </c>
       <c r="G280" t="s">
-        <v>1113</v>
+        <v>1121</v>
       </c>
       <c r="H280">
         <v>0.8</v>
@@ -14419,21 +14476,21 @@
         <v>0.95420000000000005</v>
       </c>
       <c r="J280" t="s">
-        <v>1114</v>
+        <v>1122</v>
       </c>
       <c r="K280">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="281" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12">
       <c r="A281" t="s">
-        <v>1115</v>
+        <v>1123</v>
       </c>
       <c r="B281" t="s">
-        <v>1116</v>
+        <v>1124</v>
       </c>
       <c r="C281" t="s">
-        <v>1117</v>
+        <v>1125</v>
       </c>
       <c r="D281">
         <v>0</v>
@@ -14445,7 +14502,7 @@
         <v>0.95888877000712913</v>
       </c>
       <c r="G281" t="s">
-        <v>1118</v>
+        <v>1126</v>
       </c>
       <c r="H281">
         <v>0.94</v>
@@ -14454,21 +14511,21 @@
         <v>0.97930000000000006</v>
       </c>
       <c r="J281" t="s">
-        <v>1119</v>
+        <v>1127</v>
       </c>
       <c r="K281">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="282" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12">
       <c r="A282" t="s">
-        <v>1120</v>
+        <v>1128</v>
       </c>
       <c r="B282" t="s">
-        <v>1121</v>
+        <v>1129</v>
       </c>
       <c r="C282" t="s">
-        <v>1122</v>
+        <v>1130</v>
       </c>
       <c r="D282">
         <v>0</v>
@@ -14480,7 +14537,7 @@
         <v>0.7648210692727796</v>
       </c>
       <c r="G282" t="s">
-        <v>1123</v>
+        <v>1131</v>
       </c>
       <c r="H282">
         <v>0.45</v>
@@ -14489,21 +14546,24 @@
         <v>0.79579999999999995</v>
       </c>
       <c r="J282" t="s">
-        <v>1124</v>
+        <v>1132</v>
       </c>
       <c r="K282">
         <v>0</v>
       </c>
-    </row>
-    <row r="283" spans="1:11">
+      <c r="L282" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12">
       <c r="A283" t="s">
-        <v>1125</v>
+        <v>1134</v>
       </c>
       <c r="B283" t="s">
-        <v>1126</v>
+        <v>1135</v>
       </c>
       <c r="C283" t="s">
-        <v>1127</v>
+        <v>1136</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -14515,7 +14575,7 @@
         <v>0.51308676160337541</v>
       </c>
       <c r="G283" t="s">
-        <v>1128</v>
+        <v>1137</v>
       </c>
       <c r="H283">
         <v>0.24</v>
@@ -14524,21 +14584,21 @@
         <v>0.80349999999999999</v>
       </c>
       <c r="J283" t="s">
-        <v>1129</v>
+        <v>1138</v>
       </c>
       <c r="K283">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12">
       <c r="A284" t="s">
-        <v>1130</v>
+        <v>1139</v>
       </c>
       <c r="B284" t="s">
-        <v>1131</v>
+        <v>1140</v>
       </c>
       <c r="C284" t="s">
-        <v>1132</v>
+        <v>1141</v>
       </c>
       <c r="D284">
         <v>0</v>
@@ -14550,7 +14610,7 @@
         <v>0.7903310628307747</v>
       </c>
       <c r="G284" t="s">
-        <v>1133</v>
+        <v>1142</v>
       </c>
       <c r="H284">
         <v>0.63</v>
@@ -14559,21 +14619,21 @@
         <v>0.87690000000000001</v>
       </c>
       <c r="J284" t="s">
-        <v>1134</v>
+        <v>1143</v>
       </c>
       <c r="K284">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="285" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12">
       <c r="A285" t="s">
-        <v>1135</v>
+        <v>1144</v>
       </c>
       <c r="B285" t="s">
-        <v>1136</v>
+        <v>1145</v>
       </c>
       <c r="C285" t="s">
-        <v>1137</v>
+        <v>1146</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -14597,18 +14657,18 @@
         <v>132</v>
       </c>
       <c r="K285">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="286" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12">
       <c r="A286" t="s">
-        <v>1138</v>
+        <v>1147</v>
       </c>
       <c r="B286" t="s">
-        <v>1139</v>
+        <v>1148</v>
       </c>
       <c r="C286" t="s">
-        <v>1140</v>
+        <v>1149</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -14629,21 +14689,21 @@
         <v>0.92989999999999995</v>
       </c>
       <c r="J286" t="s">
-        <v>1141</v>
+        <v>1150</v>
       </c>
       <c r="K286">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12">
       <c r="A287" t="s">
-        <v>1142</v>
+        <v>1151</v>
       </c>
       <c r="B287" t="s">
-        <v>1143</v>
+        <v>1152</v>
       </c>
       <c r="C287" t="s">
-        <v>1144</v>
+        <v>1153</v>
       </c>
       <c r="D287">
         <v>0</v>
@@ -14655,7 +14715,7 @@
         <v>0.99993750000000003</v>
       </c>
       <c r="G287" t="s">
-        <v>1145</v>
+        <v>1154</v>
       </c>
       <c r="H287">
         <v>0.91</v>
@@ -14664,21 +14724,21 @@
         <v>0.98349999999999993</v>
       </c>
       <c r="J287" t="s">
-        <v>1146</v>
+        <v>1155</v>
       </c>
       <c r="K287">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12">
       <c r="A288" t="s">
-        <v>1147</v>
+        <v>1156</v>
       </c>
       <c r="B288" t="s">
-        <v>1148</v>
+        <v>1157</v>
       </c>
       <c r="C288" t="s">
-        <v>1149</v>
+        <v>1158</v>
       </c>
       <c r="D288">
         <v>0</v>
@@ -14690,7 +14750,7 @@
         <v>0.82735042735042752</v>
       </c>
       <c r="G288" t="s">
-        <v>1150</v>
+        <v>1159</v>
       </c>
       <c r="H288">
         <v>0.3</v>
@@ -14699,21 +14759,24 @@
         <v>0.63190000000000002</v>
       </c>
       <c r="J288" t="s">
-        <v>1151</v>
+        <v>1160</v>
       </c>
       <c r="K288">
         <v>0</v>
+      </c>
+      <c r="L288" t="s">
+        <v>1161</v>
       </c>
     </row>
     <row r="289" spans="1:11">
       <c r="A289" t="s">
-        <v>1152</v>
+        <v>1162</v>
       </c>
       <c r="B289" t="s">
-        <v>1153</v>
+        <v>1163</v>
       </c>
       <c r="C289" t="s">
-        <v>1154</v>
+        <v>1164</v>
       </c>
       <c r="D289">
         <v>0</v>
@@ -14725,7 +14788,7 @@
         <v>0.97554878048780491</v>
       </c>
       <c r="G289" t="s">
-        <v>1155</v>
+        <v>1165</v>
       </c>
       <c r="H289">
         <v>0.89</v>
@@ -14734,21 +14797,21 @@
         <v>0.96530000000000005</v>
       </c>
       <c r="J289" t="s">
-        <v>1156</v>
+        <v>1166</v>
       </c>
       <c r="K289">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="290" spans="1:11">
       <c r="A290" t="s">
-        <v>1157</v>
+        <v>1167</v>
       </c>
       <c r="B290" t="s">
-        <v>1158</v>
+        <v>1168</v>
       </c>
       <c r="C290" t="s">
-        <v>1159</v>
+        <v>1169</v>
       </c>
       <c r="D290">
         <v>0</v>
@@ -14760,7 +14823,7 @@
         <v>0.9003281771919136</v>
       </c>
       <c r="G290" t="s">
-        <v>1160</v>
+        <v>1170</v>
       </c>
       <c r="H290">
         <v>0.64</v>
@@ -14769,21 +14832,21 @@
         <v>0.8417</v>
       </c>
       <c r="J290" t="s">
-        <v>1161</v>
+        <v>1171</v>
       </c>
       <c r="K290">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="291" spans="1:11">
       <c r="A291" t="s">
-        <v>1162</v>
+        <v>1172</v>
       </c>
       <c r="B291" t="s">
-        <v>1163</v>
+        <v>1173</v>
       </c>
       <c r="C291" t="s">
-        <v>1164</v>
+        <v>1174</v>
       </c>
       <c r="D291">
         <v>0</v>
@@ -14795,7 +14858,7 @@
         <v>0.93197278911564618</v>
       </c>
       <c r="G291" t="s">
-        <v>1165</v>
+        <v>1175</v>
       </c>
       <c r="H291">
         <v>0.69</v>
@@ -14812,13 +14875,13 @@
     </row>
     <row r="292" spans="1:11">
       <c r="A292" t="s">
-        <v>1166</v>
+        <v>1176</v>
       </c>
       <c r="B292" t="s">
-        <v>1167</v>
+        <v>1177</v>
       </c>
       <c r="C292" t="s">
-        <v>1168</v>
+        <v>1178</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -14830,7 +14893,7 @@
         <v>0.65260257994526893</v>
       </c>
       <c r="G292" t="s">
-        <v>1169</v>
+        <v>1179</v>
       </c>
       <c r="H292">
         <v>0.34</v>
@@ -14839,7 +14902,7 @@
         <v>0.74900000000000011</v>
       </c>
       <c r="J292" t="s">
-        <v>1170</v>
+        <v>1180</v>
       </c>
       <c r="K292">
         <v>0</v>
@@ -14847,13 +14910,13 @@
     </row>
     <row r="293" spans="1:11">
       <c r="A293" t="s">
-        <v>1171</v>
+        <v>1181</v>
       </c>
       <c r="B293" t="s">
-        <v>1172</v>
+        <v>1182</v>
       </c>
       <c r="C293" t="s">
-        <v>1173</v>
+        <v>1183</v>
       </c>
       <c r="D293">
         <v>0</v>
@@ -14865,7 +14928,7 @@
         <v>0.91703661742883691</v>
       </c>
       <c r="G293" t="s">
-        <v>1174</v>
+        <v>1184</v>
       </c>
       <c r="H293">
         <v>1</v>
@@ -14874,7 +14937,7 @@
         <v>0.94</v>
       </c>
       <c r="J293" t="s">
-        <v>1175</v>
+        <v>1185</v>
       </c>
       <c r="K293">
         <v>0</v>
@@ -14882,13 +14945,13 @@
     </row>
     <row r="294" spans="1:11">
       <c r="A294" t="s">
-        <v>1176</v>
+        <v>1186</v>
       </c>
       <c r="B294" t="s">
-        <v>1177</v>
+        <v>1187</v>
       </c>
       <c r="C294" t="s">
-        <v>1178</v>
+        <v>1188</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -14900,7 +14963,7 @@
         <v>0.73776919828678289</v>
       </c>
       <c r="G294" t="s">
-        <v>1179</v>
+        <v>1189</v>
       </c>
       <c r="H294">
         <v>0.62</v>
@@ -14909,7 +14972,7 @@
         <v>0.80400000000000005</v>
       </c>
       <c r="J294" t="s">
-        <v>1180</v>
+        <v>1190</v>
       </c>
       <c r="K294">
         <v>0</v>
@@ -14917,13 +14980,13 @@
     </row>
     <row r="295" spans="1:11">
       <c r="A295" t="s">
-        <v>1181</v>
+        <v>1191</v>
       </c>
       <c r="B295" t="s">
-        <v>1182</v>
+        <v>1192</v>
       </c>
       <c r="C295" t="s">
-        <v>1183</v>
+        <v>1193</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -14935,7 +14998,7 @@
         <v>0.89711883308721962</v>
       </c>
       <c r="G295" t="s">
-        <v>1184</v>
+        <v>1194</v>
       </c>
       <c r="H295">
         <v>0.75</v>
@@ -14944,7 +15007,7 @@
         <v>0.93019999999999992</v>
       </c>
       <c r="J295" t="s">
-        <v>1185</v>
+        <v>1195</v>
       </c>
       <c r="K295">
         <v>0</v>
@@ -14952,13 +15015,13 @@
     </row>
     <row r="296" spans="1:11">
       <c r="A296" t="s">
-        <v>1186</v>
+        <v>1196</v>
       </c>
       <c r="B296" t="s">
-        <v>1187</v>
+        <v>1197</v>
       </c>
       <c r="C296" t="s">
-        <v>1188</v>
+        <v>1198</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -14970,7 +15033,7 @@
         <v>0.79250589368334379</v>
       </c>
       <c r="G296" t="s">
-        <v>1189</v>
+        <v>1199</v>
       </c>
       <c r="H296">
         <v>0.71</v>
@@ -14979,7 +15042,7 @@
         <v>0.91689999999999994</v>
       </c>
       <c r="J296" t="s">
-        <v>1190</v>
+        <v>1200</v>
       </c>
       <c r="K296">
         <v>0</v>
@@ -14987,13 +15050,13 @@
     </row>
     <row r="297" spans="1:11">
       <c r="A297" t="s">
-        <v>1191</v>
+        <v>1201</v>
       </c>
       <c r="B297" t="s">
-        <v>1192</v>
+        <v>1202</v>
       </c>
       <c r="C297" t="s">
-        <v>1192</v>
+        <v>1202</v>
       </c>
       <c r="D297">
         <v>1</v>
@@ -15022,13 +15085,13 @@
     </row>
     <row r="298" spans="1:11">
       <c r="A298" t="s">
-        <v>1193</v>
+        <v>1203</v>
       </c>
       <c r="B298" t="s">
-        <v>1194</v>
+        <v>1204</v>
       </c>
       <c r="C298" t="s">
-        <v>1195</v>
+        <v>1205</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -15040,7 +15103,7 @@
         <v>0.99735703251328245</v>
       </c>
       <c r="G298" t="s">
-        <v>1196</v>
+        <v>1206</v>
       </c>
       <c r="H298">
         <v>0.9</v>
@@ -15049,7 +15112,7 @@
         <v>0.95909999999999995</v>
       </c>
       <c r="J298" t="s">
-        <v>1197</v>
+        <v>1207</v>
       </c>
       <c r="K298">
         <v>0</v>
@@ -15057,13 +15120,13 @@
     </row>
     <row r="299" spans="1:11">
       <c r="A299" t="s">
-        <v>1198</v>
+        <v>1208</v>
       </c>
       <c r="B299" t="s">
-        <v>1199</v>
+        <v>1209</v>
       </c>
       <c r="C299" t="s">
-        <v>1200</v>
+        <v>1210</v>
       </c>
       <c r="D299">
         <v>0</v>
@@ -15075,7 +15138,7 @@
         <v>0.85687569193583235</v>
       </c>
       <c r="G299" t="s">
-        <v>1201</v>
+        <v>1211</v>
       </c>
       <c r="H299">
         <v>0.79</v>
@@ -15084,7 +15147,7 @@
         <v>0.98640000000000005</v>
       </c>
       <c r="J299" t="s">
-        <v>1202</v>
+        <v>1212</v>
       </c>
       <c r="K299">
         <v>0</v>
@@ -15092,13 +15155,13 @@
     </row>
     <row r="300" spans="1:11">
       <c r="A300" t="s">
-        <v>1203</v>
+        <v>1213</v>
       </c>
       <c r="B300" t="s">
-        <v>1204</v>
+        <v>1214</v>
       </c>
       <c r="C300" t="s">
-        <v>1205</v>
+        <v>1215</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -15110,7 +15173,7 @@
         <v>0.86221105326895342</v>
       </c>
       <c r="G300" t="s">
-        <v>1206</v>
+        <v>1216</v>
       </c>
       <c r="H300">
         <v>0.71</v>
@@ -15119,7 +15182,7 @@
         <v>0.93730000000000002</v>
       </c>
       <c r="J300" t="s">
-        <v>1207</v>
+        <v>1217</v>
       </c>
       <c r="K300">
         <v>0</v>
@@ -15127,13 +15190,13 @@
     </row>
     <row r="301" spans="1:11">
       <c r="A301" t="s">
-        <v>1208</v>
+        <v>1218</v>
       </c>
       <c r="B301" t="s">
-        <v>1209</v>
+        <v>1219</v>
       </c>
       <c r="C301" t="s">
-        <v>1210</v>
+        <v>1220</v>
       </c>
       <c r="D301">
         <v>0</v>
@@ -15145,7 +15208,7 @@
         <v>0.99610749193911696</v>
       </c>
       <c r="G301" t="s">
-        <v>1211</v>
+        <v>1221</v>
       </c>
       <c r="H301">
         <v>0.85</v>
@@ -15154,7 +15217,7 @@
         <v>0.96879999999999999</v>
       </c>
       <c r="J301" t="s">
-        <v>1212</v>
+        <v>1222</v>
       </c>
       <c r="K301">
         <v>0</v>
@@ -15162,13 +15225,13 @@
     </row>
     <row r="302" spans="1:11">
       <c r="A302" t="s">
-        <v>1213</v>
+        <v>1223</v>
       </c>
       <c r="B302" t="s">
-        <v>1214</v>
+        <v>1224</v>
       </c>
       <c r="C302" t="s">
-        <v>1215</v>
+        <v>1225</v>
       </c>
       <c r="D302">
         <v>0</v>
@@ -15180,7 +15243,7 @@
         <v>0.78805201069249298</v>
       </c>
       <c r="G302" t="s">
-        <v>1216</v>
+        <v>1226</v>
       </c>
       <c r="H302">
         <v>0.7</v>
@@ -15189,7 +15252,7 @@
         <v>0.93129999999999991</v>
       </c>
       <c r="J302" t="s">
-        <v>1217</v>
+        <v>1227</v>
       </c>
       <c r="K302">
         <v>0</v>
@@ -15197,13 +15260,13 @@
     </row>
     <row r="303" spans="1:11">
       <c r="A303" t="s">
-        <v>1218</v>
+        <v>1228</v>
       </c>
       <c r="B303" t="s">
-        <v>1219</v>
+        <v>1229</v>
       </c>
       <c r="C303" t="s">
-        <v>1220</v>
+        <v>1230</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -15215,7 +15278,7 @@
         <v>0.96943863981762923</v>
       </c>
       <c r="G303" t="s">
-        <v>1221</v>
+        <v>1231</v>
       </c>
       <c r="H303">
         <v>0.39</v>
@@ -15224,7 +15287,7 @@
         <v>0.8</v>
       </c>
       <c r="J303" t="s">
-        <v>1222</v>
+        <v>1232</v>
       </c>
       <c r="K303">
         <v>0</v>
@@ -15232,13 +15295,13 @@
     </row>
     <row r="304" spans="1:11">
       <c r="A304" t="s">
-        <v>1223</v>
+        <v>1233</v>
       </c>
       <c r="B304" t="s">
-        <v>1224</v>
+        <v>1234</v>
       </c>
       <c r="C304" t="s">
-        <v>1225</v>
+        <v>1235</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -15250,7 +15313,7 @@
         <v>0.93118385612182153</v>
       </c>
       <c r="G304" t="s">
-        <v>1226</v>
+        <v>1236</v>
       </c>
       <c r="H304">
         <v>1</v>
@@ -15259,7 +15322,7 @@
         <v>0.97329999999999994</v>
       </c>
       <c r="J304" t="s">
-        <v>1227</v>
+        <v>1237</v>
       </c>
       <c r="K304">
         <v>0</v>
@@ -15267,13 +15330,13 @@
     </row>
     <row r="305" spans="1:11">
       <c r="A305" t="s">
-        <v>1228</v>
+        <v>1238</v>
       </c>
       <c r="B305" t="s">
-        <v>1229</v>
+        <v>1239</v>
       </c>
       <c r="C305" t="s">
-        <v>1230</v>
+        <v>1240</v>
       </c>
       <c r="D305">
         <v>0</v>
@@ -15285,7 +15348,7 @@
         <v>0.92150987268919982</v>
       </c>
       <c r="G305" t="s">
-        <v>1231</v>
+        <v>1241</v>
       </c>
       <c r="H305">
         <v>0.73</v>
@@ -15294,7 +15357,7 @@
         <v>0.86599999999999999</v>
       </c>
       <c r="J305" t="s">
-        <v>1232</v>
+        <v>1242</v>
       </c>
       <c r="K305">
         <v>0</v>
@@ -15302,13 +15365,13 @@
     </row>
     <row r="306" spans="1:11">
       <c r="A306" t="s">
-        <v>1233</v>
+        <v>1243</v>
       </c>
       <c r="B306" t="s">
-        <v>1234</v>
+        <v>1244</v>
       </c>
       <c r="C306" t="s">
-        <v>1234</v>
+        <v>1244</v>
       </c>
       <c r="D306">
         <v>1</v>
@@ -15337,13 +15400,13 @@
     </row>
     <row r="307" spans="1:11">
       <c r="A307" t="s">
-        <v>1235</v>
+        <v>1245</v>
       </c>
       <c r="B307" t="s">
-        <v>1236</v>
+        <v>1246</v>
       </c>
       <c r="C307" t="s">
-        <v>1237</v>
+        <v>1247</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -15355,7 +15418,7 @@
         <v>0.84459459459459441</v>
       </c>
       <c r="G307" t="s">
-        <v>1238</v>
+        <v>1248</v>
       </c>
       <c r="H307">
         <v>0.62</v>
@@ -15364,7 +15427,7 @@
         <v>0.95609999999999995</v>
       </c>
       <c r="J307" t="s">
-        <v>1239</v>
+        <v>1249</v>
       </c>
       <c r="K307">
         <v>0</v>
@@ -15372,13 +15435,13 @@
     </row>
     <row r="308" spans="1:11">
       <c r="A308" t="s">
-        <v>1240</v>
+        <v>1250</v>
       </c>
       <c r="B308" t="s">
-        <v>1241</v>
+        <v>1251</v>
       </c>
       <c r="C308" t="s">
-        <v>1242</v>
+        <v>1252</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -15390,7 +15453,7 @@
         <v>0.88969017094017089</v>
       </c>
       <c r="G308" t="s">
-        <v>1243</v>
+        <v>1253</v>
       </c>
       <c r="H308">
         <v>0.52</v>
@@ -15399,7 +15462,7 @@
         <v>0.79569999999999996</v>
       </c>
       <c r="J308" t="s">
-        <v>1244</v>
+        <v>1254</v>
       </c>
       <c r="K308">
         <v>0</v>
@@ -15407,13 +15470,13 @@
     </row>
     <row r="309" spans="1:11">
       <c r="A309" t="s">
-        <v>1245</v>
+        <v>1255</v>
       </c>
       <c r="B309" t="s">
-        <v>1246</v>
+        <v>1256</v>
       </c>
       <c r="C309" t="s">
-        <v>1247</v>
+        <v>1257</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -15425,7 +15488,7 @@
         <v>0.91395863315515335</v>
       </c>
       <c r="G309" t="s">
-        <v>1248</v>
+        <v>1258</v>
       </c>
       <c r="H309">
         <v>0.71</v>
@@ -15434,7 +15497,7 @@
         <v>0.9173</v>
       </c>
       <c r="J309" t="s">
-        <v>1249</v>
+        <v>1259</v>
       </c>
       <c r="K309">
         <v>0</v>
@@ -15442,13 +15505,13 @@
     </row>
     <row r="310" spans="1:11">
       <c r="A310" t="s">
-        <v>1250</v>
+        <v>1260</v>
       </c>
       <c r="B310" t="s">
-        <v>1251</v>
+        <v>1261</v>
       </c>
       <c r="C310" t="s">
-        <v>1251</v>
+        <v>1261</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -15477,13 +15540,13 @@
     </row>
     <row r="311" spans="1:11">
       <c r="A311" t="s">
-        <v>1252</v>
+        <v>1262</v>
       </c>
       <c r="B311" t="s">
-        <v>1253</v>
+        <v>1263</v>
       </c>
       <c r="C311" t="s">
-        <v>1254</v>
+        <v>1264</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -15495,7 +15558,7 @@
         <v>0.58455728246307592</v>
       </c>
       <c r="G311" t="s">
-        <v>1255</v>
+        <v>1265</v>
       </c>
       <c r="H311">
         <v>0.22</v>
@@ -15504,7 +15567,7 @@
         <v>0.86419999999999997</v>
       </c>
       <c r="J311" t="s">
-        <v>1256</v>
+        <v>1266</v>
       </c>
       <c r="K311">
         <v>0</v>
@@ -15512,13 +15575,13 @@
     </row>
     <row r="312" spans="1:11">
       <c r="A312" t="s">
-        <v>1257</v>
+        <v>1267</v>
       </c>
       <c r="B312" t="s">
-        <v>1258</v>
+        <v>1268</v>
       </c>
       <c r="C312" t="s">
-        <v>1259</v>
+        <v>1269</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -15530,7 +15593,7 @@
         <v>0.96341746046674104</v>
       </c>
       <c r="G312" t="s">
-        <v>1260</v>
+        <v>1270</v>
       </c>
       <c r="H312">
         <v>0.82</v>
@@ -15539,7 +15602,7 @@
         <v>0.9375</v>
       </c>
       <c r="J312" t="s">
-        <v>1261</v>
+        <v>1271</v>
       </c>
       <c r="K312">
         <v>0</v>
@@ -15547,13 +15610,13 @@
     </row>
     <row r="313" spans="1:11">
       <c r="A313" t="s">
-        <v>1262</v>
+        <v>1272</v>
       </c>
       <c r="B313" t="s">
-        <v>1263</v>
+        <v>1273</v>
       </c>
       <c r="C313" t="s">
-        <v>1264</v>
+        <v>1274</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -15565,7 +15628,7 @@
         <v>0.78049017672603971</v>
       </c>
       <c r="G313" t="s">
-        <v>1265</v>
+        <v>1275</v>
       </c>
       <c r="H313">
         <v>0.84</v>
@@ -15574,7 +15637,7 @@
         <v>0.94830000000000003</v>
       </c>
       <c r="J313" t="s">
-        <v>1266</v>
+        <v>1276</v>
       </c>
       <c r="K313">
         <v>0</v>
@@ -15582,13 +15645,13 @@
     </row>
     <row r="314" spans="1:11">
       <c r="A314" t="s">
-        <v>1267</v>
+        <v>1277</v>
       </c>
       <c r="B314" t="s">
-        <v>1268</v>
+        <v>1278</v>
       </c>
       <c r="C314" t="s">
-        <v>1269</v>
+        <v>1279</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -15600,7 +15663,7 @@
         <v>0.90394202898550713</v>
       </c>
       <c r="G314" t="s">
-        <v>1270</v>
+        <v>1280</v>
       </c>
       <c r="H314">
         <v>0.92</v>
@@ -15609,7 +15672,7 @@
         <v>0.96870000000000001</v>
       </c>
       <c r="J314" t="s">
-        <v>1271</v>
+        <v>1281</v>
       </c>
       <c r="K314">
         <v>0</v>
@@ -15617,13 +15680,13 @@
     </row>
     <row r="315" spans="1:11">
       <c r="A315" t="s">
-        <v>1272</v>
+        <v>1282</v>
       </c>
       <c r="B315" t="s">
-        <v>1273</v>
+        <v>1283</v>
       </c>
       <c r="C315" t="s">
-        <v>1274</v>
+        <v>1284</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -15635,7 +15698,7 @@
         <v>0.87517556179775269</v>
       </c>
       <c r="G315" t="s">
-        <v>1275</v>
+        <v>1285</v>
       </c>
       <c r="H315">
         <v>0.5</v>
@@ -15652,13 +15715,13 @@
     </row>
     <row r="316" spans="1:11">
       <c r="A316" t="s">
-        <v>1276</v>
+        <v>1286</v>
       </c>
       <c r="B316" t="s">
-        <v>1277</v>
+        <v>1287</v>
       </c>
       <c r="C316" t="s">
-        <v>1278</v>
+        <v>1288</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -15670,7 +15733,7 @@
         <v>0.77401692384270782</v>
       </c>
       <c r="G316" t="s">
-        <v>1279</v>
+        <v>1289</v>
       </c>
       <c r="H316">
         <v>0.49</v>
@@ -15679,7 +15742,7 @@
         <v>0.88280000000000003</v>
       </c>
       <c r="J316" t="s">
-        <v>1280</v>
+        <v>1290</v>
       </c>
       <c r="K316">
         <v>0</v>
@@ -15687,13 +15750,13 @@
     </row>
     <row r="317" spans="1:11">
       <c r="A317" t="s">
-        <v>1281</v>
+        <v>1291</v>
       </c>
       <c r="B317" t="s">
-        <v>1282</v>
+        <v>1292</v>
       </c>
       <c r="C317" t="s">
-        <v>1283</v>
+        <v>1293</v>
       </c>
       <c r="D317">
         <v>0</v>
@@ -15705,7 +15768,7 @@
         <v>0.70448824816204658</v>
       </c>
       <c r="G317" t="s">
-        <v>1284</v>
+        <v>1294</v>
       </c>
       <c r="H317">
         <v>0.53</v>
@@ -15714,7 +15777,7 @@
         <v>0.9103</v>
       </c>
       <c r="J317" t="s">
-        <v>1285</v>
+        <v>1295</v>
       </c>
       <c r="K317">
         <v>0</v>
@@ -15722,13 +15785,13 @@
     </row>
     <row r="318" spans="1:11">
       <c r="A318" t="s">
-        <v>1286</v>
+        <v>1296</v>
       </c>
       <c r="B318" t="s">
-        <v>1287</v>
+        <v>1297</v>
       </c>
       <c r="C318" t="s">
-        <v>1288</v>
+        <v>1298</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -15740,7 +15803,7 @@
         <v>0.8578868267449582</v>
       </c>
       <c r="G318" t="s">
-        <v>1289</v>
+        <v>1299</v>
       </c>
       <c r="H318">
         <v>1</v>
@@ -15749,7 +15812,7 @@
         <v>0.93700000000000006</v>
       </c>
       <c r="J318" t="s">
-        <v>1290</v>
+        <v>1300</v>
       </c>
       <c r="K318">
         <v>0</v>
@@ -15757,13 +15820,13 @@
     </row>
     <row r="319" spans="1:11">
       <c r="A319" t="s">
-        <v>1291</v>
+        <v>1301</v>
       </c>
       <c r="B319" t="s">
-        <v>1292</v>
+        <v>1302</v>
       </c>
       <c r="C319" t="s">
-        <v>1293</v>
+        <v>1303</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -15775,7 +15838,7 @@
         <v>0.98576950809165209</v>
       </c>
       <c r="G319" t="s">
-        <v>1294</v>
+        <v>1304</v>
       </c>
       <c r="H319">
         <v>0.91</v>
@@ -15784,7 +15847,7 @@
         <v>0.96109999999999995</v>
       </c>
       <c r="J319" t="s">
-        <v>1295</v>
+        <v>1305</v>
       </c>
       <c r="K319">
         <v>0</v>
@@ -15792,13 +15855,13 @@
     </row>
     <row r="320" spans="1:11">
       <c r="A320" t="s">
-        <v>1296</v>
+        <v>1306</v>
       </c>
       <c r="B320" t="s">
-        <v>1297</v>
+        <v>1307</v>
       </c>
       <c r="C320" t="s">
-        <v>1298</v>
+        <v>1308</v>
       </c>
       <c r="D320">
         <v>0</v>
@@ -15810,7 +15873,7 @@
         <v>0.99142030393168623</v>
       </c>
       <c r="G320" t="s">
-        <v>1299</v>
+        <v>1309</v>
       </c>
       <c r="H320">
         <v>0.84</v>
@@ -15827,13 +15890,13 @@
     </row>
     <row r="321" spans="1:11">
       <c r="A321" t="s">
-        <v>1300</v>
+        <v>1310</v>
       </c>
       <c r="B321" t="s">
-        <v>1301</v>
+        <v>1311</v>
       </c>
       <c r="C321" t="s">
-        <v>1301</v>
+        <v>1311</v>
       </c>
       <c r="D321">
         <v>1</v>
@@ -15862,13 +15925,13 @@
     </row>
     <row r="322" spans="1:11">
       <c r="A322" t="s">
-        <v>1302</v>
+        <v>1312</v>
       </c>
       <c r="B322" t="s">
-        <v>1303</v>
+        <v>1313</v>
       </c>
       <c r="C322" t="s">
-        <v>1304</v>
+        <v>1314</v>
       </c>
       <c r="D322">
         <v>0</v>
@@ -15880,7 +15943,7 @@
         <v>0.95990232827825017</v>
       </c>
       <c r="G322" t="s">
-        <v>1305</v>
+        <v>1315</v>
       </c>
       <c r="H322">
         <v>0.59</v>
@@ -15889,7 +15952,7 @@
         <v>0.8427</v>
       </c>
       <c r="J322" t="s">
-        <v>1306</v>
+        <v>1316</v>
       </c>
       <c r="K322">
         <v>0</v>
@@ -15897,13 +15960,13 @@
     </row>
     <row r="323" spans="1:11">
       <c r="A323" t="s">
-        <v>1307</v>
+        <v>1317</v>
       </c>
       <c r="B323" t="s">
-        <v>1308</v>
+        <v>1318</v>
       </c>
       <c r="C323" t="s">
-        <v>1309</v>
+        <v>1319</v>
       </c>
       <c r="D323">
         <v>0</v>
@@ -15915,7 +15978,7 @@
         <v>0.91487850396871861</v>
       </c>
       <c r="G323" t="s">
-        <v>1310</v>
+        <v>1320</v>
       </c>
       <c r="H323">
         <v>0.88</v>
@@ -15924,7 +15987,7 @@
         <v>0.95950000000000002</v>
       </c>
       <c r="J323" t="s">
-        <v>1311</v>
+        <v>1321</v>
       </c>
       <c r="K323">
         <v>0</v>
@@ -15932,13 +15995,13 @@
     </row>
     <row r="324" spans="1:11">
       <c r="A324" t="s">
-        <v>1312</v>
+        <v>1322</v>
       </c>
       <c r="B324" t="s">
-        <v>1313</v>
+        <v>1323</v>
       </c>
       <c r="C324" t="s">
-        <v>1314</v>
+        <v>1324</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -15950,7 +16013,7 @@
         <v>0.84168421052631581</v>
       </c>
       <c r="G324" t="s">
-        <v>1315</v>
+        <v>1325</v>
       </c>
       <c r="H324">
         <v>0.62</v>
@@ -15959,7 +16022,7 @@
         <v>0.92590000000000006</v>
       </c>
       <c r="J324" t="s">
-        <v>1261</v>
+        <v>1271</v>
       </c>
       <c r="K324">
         <v>0</v>
@@ -15967,13 +16030,13 @@
     </row>
     <row r="325" spans="1:11">
       <c r="A325" t="s">
-        <v>1316</v>
+        <v>1326</v>
       </c>
       <c r="B325" t="s">
-        <v>1317</v>
+        <v>1327</v>
       </c>
       <c r="C325" t="s">
-        <v>1318</v>
+        <v>1328</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -15985,7 +16048,7 @@
         <v>0.89947226617328602</v>
       </c>
       <c r="G325" t="s">
-        <v>1319</v>
+        <v>1329</v>
       </c>
       <c r="H325">
         <v>0.74</v>
@@ -15994,7 +16057,7 @@
         <v>0.93849999999999989</v>
       </c>
       <c r="J325" t="s">
-        <v>1320</v>
+        <v>1330</v>
       </c>
       <c r="K325">
         <v>1</v>
@@ -16002,13 +16065,13 @@
     </row>
     <row r="326" spans="1:11">
       <c r="A326" t="s">
-        <v>1321</v>
+        <v>1331</v>
       </c>
       <c r="B326" t="s">
-        <v>1322</v>
+        <v>1332</v>
       </c>
       <c r="C326" t="s">
-        <v>1323</v>
+        <v>1333</v>
       </c>
       <c r="D326">
         <v>0</v>
@@ -16020,7 +16083,7 @@
         <v>0.98131106566689386</v>
       </c>
       <c r="G326" t="s">
-        <v>1324</v>
+        <v>1334</v>
       </c>
       <c r="H326">
         <v>0.92</v>
@@ -16029,7 +16092,7 @@
         <v>0.98769999999999991</v>
       </c>
       <c r="J326" t="s">
-        <v>1325</v>
+        <v>1335</v>
       </c>
       <c r="K326">
         <v>1</v>
@@ -16037,13 +16100,13 @@
     </row>
     <row r="327" spans="1:11">
       <c r="A327" t="s">
-        <v>1326</v>
+        <v>1336</v>
       </c>
       <c r="B327" t="s">
-        <v>1327</v>
+        <v>1337</v>
       </c>
       <c r="C327" t="s">
-        <v>1328</v>
+        <v>1338</v>
       </c>
       <c r="D327">
         <v>0</v>
@@ -16055,7 +16118,7 @@
         <v>0.78317639673571882</v>
       </c>
       <c r="G327" t="s">
-        <v>1329</v>
+        <v>1339</v>
       </c>
       <c r="H327">
         <v>0.6</v>
@@ -16064,7 +16127,7 @@
         <v>0.7742</v>
       </c>
       <c r="J327" t="s">
-        <v>1330</v>
+        <v>1340</v>
       </c>
       <c r="K327">
         <v>1</v>

</xml_diff>

<commit_message>
Fine analisi Claude Sonnet
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiClaudeSonnet.xlsx
+++ b/HE/W_in_progress/AnalisiClaudeSonnet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{681E22F3-AB23-493F-9BEA-38F3C4F9F21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9577A65-E8BD-4A6A-99BF-6F260F68123E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="1341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="1342">
   <si>
     <t>IN</t>
   </si>
@@ -3781,6 +3781,9 @@
   </si>
   <si>
     <t>0.5217391256710776</t>
+  </si>
+  <si>
+    <t>Non da il nome al processo, ma va bene</t>
   </si>
   <si>
     <t>REVISION is a constant of type integer initialized to 0; input_mag is an instance of inputmanager with signals clock, rst, value_in t_btn_plainText, plaintext64</t>
@@ -4442,8 +4445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
-      <selection activeCell="K291" sqref="K291"/>
+    <sheetView tabSelected="1" topLeftCell="A299" workbookViewId="0">
+      <selection activeCell="L324" sqref="L324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14870,7 +14873,7 @@
         <v>543</v>
       </c>
       <c r="K291">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="292" spans="1:11">
@@ -14905,7 +14908,7 @@
         <v>1180</v>
       </c>
       <c r="K292">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="293" spans="1:11">
@@ -14940,7 +14943,7 @@
         <v>1185</v>
       </c>
       <c r="K293">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="294" spans="1:11">
@@ -14975,7 +14978,7 @@
         <v>1190</v>
       </c>
       <c r="K294">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295" spans="1:11">
@@ -15010,7 +15013,7 @@
         <v>1195</v>
       </c>
       <c r="K295">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="296" spans="1:11">
@@ -15045,7 +15048,7 @@
         <v>1200</v>
       </c>
       <c r="K296">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="297" spans="1:11">
@@ -15115,7 +15118,7 @@
         <v>1207</v>
       </c>
       <c r="K298">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="299" spans="1:11">
@@ -15150,7 +15153,7 @@
         <v>1212</v>
       </c>
       <c r="K299">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="300" spans="1:11">
@@ -15185,7 +15188,7 @@
         <v>1217</v>
       </c>
       <c r="K300">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="301" spans="1:11">
@@ -15220,7 +15223,7 @@
         <v>1222</v>
       </c>
       <c r="K301">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="302" spans="1:11">
@@ -15255,7 +15258,7 @@
         <v>1227</v>
       </c>
       <c r="K302">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="303" spans="1:11">
@@ -15290,7 +15293,7 @@
         <v>1232</v>
       </c>
       <c r="K303">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="304" spans="1:11">
@@ -15325,10 +15328,10 @@
         <v>1237</v>
       </c>
       <c r="K304">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="305" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12">
       <c r="A305" t="s">
         <v>1238</v>
       </c>
@@ -15360,10 +15363,10 @@
         <v>1242</v>
       </c>
       <c r="K305">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="306" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:12">
       <c r="A306" t="s">
         <v>1243</v>
       </c>
@@ -15398,7 +15401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:11">
+    <row r="307" spans="1:12">
       <c r="A307" t="s">
         <v>1245</v>
       </c>
@@ -15430,18 +15433,21 @@
         <v>1249</v>
       </c>
       <c r="K307">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="308" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L307" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="308" spans="1:12">
       <c r="A308" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="B308" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="C308" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -15453,7 +15459,7 @@
         <v>0.88969017094017089</v>
       </c>
       <c r="G308" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="H308">
         <v>0.52</v>
@@ -15462,21 +15468,21 @@
         <v>0.79569999999999996</v>
       </c>
       <c r="J308" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="K308">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="309" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12">
       <c r="A309" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="B309" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="C309" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -15488,7 +15494,7 @@
         <v>0.91395863315515335</v>
       </c>
       <c r="G309" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="H309">
         <v>0.71</v>
@@ -15497,21 +15503,21 @@
         <v>0.9173</v>
       </c>
       <c r="J309" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="K309">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="310" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:12">
       <c r="A310" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="B310" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="C310" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -15538,15 +15544,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:11">
+    <row r="311" spans="1:12">
       <c r="A311" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="B311" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="C311" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -15558,7 +15564,7 @@
         <v>0.58455728246307592</v>
       </c>
       <c r="G311" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="H311">
         <v>0.22</v>
@@ -15567,21 +15573,21 @@
         <v>0.86419999999999997</v>
       </c>
       <c r="J311" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="K311">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="312" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:12">
       <c r="A312" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="B312" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="C312" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -15593,7 +15599,7 @@
         <v>0.96341746046674104</v>
       </c>
       <c r="G312" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="H312">
         <v>0.82</v>
@@ -15602,21 +15608,21 @@
         <v>0.9375</v>
       </c>
       <c r="J312" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="K312">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="313" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:12">
       <c r="A313" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="B313" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="C313" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -15628,7 +15634,7 @@
         <v>0.78049017672603971</v>
       </c>
       <c r="G313" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="H313">
         <v>0.84</v>
@@ -15637,21 +15643,21 @@
         <v>0.94830000000000003</v>
       </c>
       <c r="J313" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="K313">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="314" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:12">
       <c r="A314" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="B314" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="C314" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -15663,7 +15669,7 @@
         <v>0.90394202898550713</v>
       </c>
       <c r="G314" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="H314">
         <v>0.92</v>
@@ -15672,21 +15678,21 @@
         <v>0.96870000000000001</v>
       </c>
       <c r="J314" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="K314">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="315" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:12">
       <c r="A315" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="B315" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="C315" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -15698,7 +15704,7 @@
         <v>0.87517556179775269</v>
       </c>
       <c r="G315" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="H315">
         <v>0.5</v>
@@ -15710,18 +15716,21 @@
         <v>79</v>
       </c>
       <c r="K315">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="316" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L315" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="316" spans="1:12">
       <c r="A316" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="B316" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="C316" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -15733,7 +15742,7 @@
         <v>0.77401692384270782</v>
       </c>
       <c r="G316" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="H316">
         <v>0.49</v>
@@ -15742,21 +15751,21 @@
         <v>0.88280000000000003</v>
       </c>
       <c r="J316" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="K316">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="317" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:12">
       <c r="A317" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="B317" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="C317" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D317">
         <v>0</v>
@@ -15768,7 +15777,7 @@
         <v>0.70448824816204658</v>
       </c>
       <c r="G317" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="H317">
         <v>0.53</v>
@@ -15777,21 +15786,21 @@
         <v>0.9103</v>
       </c>
       <c r="J317" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="K317">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="318" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:12">
       <c r="A318" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="B318" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="C318" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -15803,7 +15812,7 @@
         <v>0.8578868267449582</v>
       </c>
       <c r="G318" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="H318">
         <v>1</v>
@@ -15812,21 +15821,21 @@
         <v>0.93700000000000006</v>
       </c>
       <c r="J318" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="K318">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="319" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:12">
       <c r="A319" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="B319" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="C319" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -15838,7 +15847,7 @@
         <v>0.98576950809165209</v>
       </c>
       <c r="G319" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="H319">
         <v>0.91</v>
@@ -15847,21 +15856,21 @@
         <v>0.96109999999999995</v>
       </c>
       <c r="J319" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="K319">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="320" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:12">
       <c r="A320" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="B320" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="C320" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D320">
         <v>0</v>
@@ -15873,7 +15882,7 @@
         <v>0.99142030393168623</v>
       </c>
       <c r="G320" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="H320">
         <v>0.84</v>
@@ -15885,18 +15894,18 @@
         <v>15</v>
       </c>
       <c r="K320">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321" spans="1:11">
       <c r="A321" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="B321" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="C321" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D321">
         <v>1</v>
@@ -15925,13 +15934,13 @@
     </row>
     <row r="322" spans="1:11">
       <c r="A322" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="B322" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="C322" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D322">
         <v>0</v>
@@ -15943,7 +15952,7 @@
         <v>0.95990232827825017</v>
       </c>
       <c r="G322" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="H322">
         <v>0.59</v>
@@ -15952,21 +15961,21 @@
         <v>0.8427</v>
       </c>
       <c r="J322" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="K322">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="323" spans="1:11">
       <c r="A323" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="B323" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="C323" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D323">
         <v>0</v>
@@ -15978,7 +15987,7 @@
         <v>0.91487850396871861</v>
       </c>
       <c r="G323" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="H323">
         <v>0.88</v>
@@ -15987,21 +15996,21 @@
         <v>0.95950000000000002</v>
       </c>
       <c r="J323" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="K323">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="324" spans="1:11">
       <c r="A324" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="B324" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="C324" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -16013,7 +16022,7 @@
         <v>0.84168421052631581</v>
       </c>
       <c r="G324" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="H324">
         <v>0.62</v>
@@ -16022,21 +16031,21 @@
         <v>0.92590000000000006</v>
       </c>
       <c r="J324" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="K324">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="325" spans="1:11">
       <c r="A325" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="B325" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="C325" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -16048,7 +16057,7 @@
         <v>0.89947226617328602</v>
       </c>
       <c r="G325" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="H325">
         <v>0.74</v>
@@ -16057,7 +16066,7 @@
         <v>0.93849999999999989</v>
       </c>
       <c r="J325" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="K325">
         <v>1</v>
@@ -16065,13 +16074,13 @@
     </row>
     <row r="326" spans="1:11">
       <c r="A326" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="B326" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="C326" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D326">
         <v>0</v>
@@ -16083,7 +16092,7 @@
         <v>0.98131106566689386</v>
       </c>
       <c r="G326" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="H326">
         <v>0.92</v>
@@ -16092,7 +16101,7 @@
         <v>0.98769999999999991</v>
       </c>
       <c r="J326" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="K326">
         <v>1</v>
@@ -16100,13 +16109,13 @@
     </row>
     <row r="327" spans="1:11">
       <c r="A327" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="B327" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="C327" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D327">
         <v>0</v>
@@ -16118,7 +16127,7 @@
         <v>0.78317639673571882</v>
       </c>
       <c r="G327" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="H327">
         <v>0.6</v>
@@ -16127,7 +16136,7 @@
         <v>0.7742</v>
       </c>
       <c r="J327" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="K327">
         <v>1</v>

</xml_diff>